<commit_message>
Fix date validation error in dashboard From/To cells
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.76461506095</v>
+        <v>46044.7671595081</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1891,7 +1891,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.76461506095</v>
+        <v>46051.7671595081</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.76461506095</v>
+        <v>46051.7671595081</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.76461506095</v>
+        <v>46046.7671595081</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2027,7 +2027,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.76461506095</v>
+        <v>46054.7671595081</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2073,7 +2073,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.76461506095</v>
+        <v>46042.7671595081</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2195,7 +2195,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.76461506095</v>
+        <v>46047.7671595081</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2269,7 +2269,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.76461506095</v>
+        <v>46052.7671595081</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.76461506095</v>
+        <v>46052.7671595081</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2335,7 +2335,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.76461506095</v>
+        <v>46039.7671595081</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2405,7 +2405,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.76461506095</v>
+        <v>46041.7671595081</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.76461506095</v>
+        <v>46041.7671595081</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.76461506095</v>
+        <v>46041.7671595081</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>
@@ -8432,7 +8432,7 @@
       <formula>$AB4="Refunded"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="17">
+  <dataValidations count="14">
     <dataValidation sqref="I4:I1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"Bangalore,Mumbai,Delhi,Hyderabad,Chennai,Pune,Other"</formula1>
     </dataValidation>
@@ -8475,18 +8475,6 @@
     <dataValidation sqref="AO4:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"Cash,UPI,Debit Card,Payment Gateway,Bank Transfer,Other"</formula1>
     </dataValidation>
-    <dataValidation sqref="Y4:Y1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" promptTitle="Select Date" prompt="Click to open calendar picker" type="date" operator="between">
-      <formula1>2020-01-01</formula1>
-      <formula2>2035-12-31</formula2>
-    </dataValidation>
-    <dataValidation sqref="AG4:AG1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" promptTitle="Select Date" prompt="Click to open calendar picker" type="date" operator="between">
-      <formula1>2020-01-01</formula1>
-      <formula2>2035-12-31</formula2>
-    </dataValidation>
-    <dataValidation sqref="AI4:AI1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" promptTitle="Select Date" prompt="Click to open calendar picker" type="date" operator="between">
-      <formula1>2020-01-01</formula1>
-      <formula2>2035-12-31</formula2>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9830,7 +9818,7 @@
       <c r="D60" s="36" t="n"/>
       <c r="F60" s="37" t="inlineStr">
         <is>
-          <t>← Click yellow cells for calendar in Google Sheets</t>
+          <t>← Type date like 17/01/2026 or 17-Jan-2026</t>
         </is>
       </c>
     </row>
@@ -9913,16 +9901,6 @@
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A1:N1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation sqref="B60" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Date" error="Please select a valid date" promptTitle="Select Date" prompt="Click to open calendar picker" type="date" operator="between">
-      <formula1>2020-01-01</formula1>
-      <formula2>2035-12-31</formula2>
-    </dataValidation>
-    <dataValidation sqref="D60" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Date" error="Please select a valid date" promptTitle="Select Date" prompt="Click to open calendar picker" type="date" operator="between">
-      <formula1>2020-01-01</formula1>
-      <formula2>2035-12-31</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Pending Balance: show 0 when Advance Status=Cleared or Payment=Received
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.7671595081</v>
+        <v>46044.76937564195</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1891,7 +1891,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.7671595081</v>
+        <v>46051.76937564195</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.7671595081</v>
+        <v>46051.76937564195</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1938,7 +1938,7 @@
         </is>
       </c>
       <c r="AL4" s="13">
-        <f>IF(X4="","",IF(AN4="Received",0,X4-IF(AJ4&lt;&gt;"",AJ4,0)))</f>
+        <f>IF(X4="","",IF(OR(AN4="Received",AK4="Cleared"),0,X4-IF(AJ4&lt;&gt;"",AJ4,0)))</f>
         <v/>
       </c>
       <c r="AM4" s="13" t="n"/>
@@ -1957,7 +1957,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.7671595081</v>
+        <v>46046.76937564195</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2027,7 +2027,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.7671595081</v>
+        <v>46054.76937564195</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
       <c r="AJ5" s="13" t="n"/>
       <c r="AK5" s="11" t="n"/>
       <c r="AL5" s="13">
-        <f>IF(X5="","",IF(AN5="Received",0,X5-IF(AJ5&lt;&gt;"",AJ5,0)))</f>
+        <f>IF(X5="","",IF(OR(AN5="Received",AK5="Cleared"),0,X5-IF(AJ5&lt;&gt;"",AJ5,0)))</f>
         <v/>
       </c>
       <c r="AM5" s="13" t="n"/>
@@ -2073,7 +2073,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.7671595081</v>
+        <v>46042.76937564195</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2176,7 +2176,7 @@
       <c r="AJ6" s="13" t="n"/>
       <c r="AK6" s="11" t="n"/>
       <c r="AL6" s="13">
-        <f>IF(X6="","",IF(AN6="Received",0,X6-IF(AJ6&lt;&gt;"",AJ6,0)))</f>
+        <f>IF(X6="","",IF(OR(AN6="Received",AK6="Cleared"),0,X6-IF(AJ6&lt;&gt;"",AJ6,0)))</f>
         <v/>
       </c>
       <c r="AM6" s="13" t="n"/>
@@ -2195,7 +2195,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.7671595081</v>
+        <v>46047.76937564195</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2269,7 +2269,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.7671595081</v>
+        <v>46052.76937564195</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.7671595081</v>
+        <v>46052.76937564195</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2316,7 +2316,7 @@
         </is>
       </c>
       <c r="AL7" s="13">
-        <f>IF(X7="","",IF(AN7="Received",0,X7-IF(AJ7&lt;&gt;"",AJ7,0)))</f>
+        <f>IF(X7="","",IF(OR(AN7="Received",AK7="Cleared"),0,X7-IF(AJ7&lt;&gt;"",AJ7,0)))</f>
         <v/>
       </c>
       <c r="AM7" s="13" t="n"/>
@@ -2335,7 +2335,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.7671595081</v>
+        <v>46039.76937564195</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2405,7 +2405,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.7671595081</v>
+        <v>46041.76937564195</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.7671595081</v>
+        <v>46041.76937564195</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.7671595081</v>
+        <v>46041.76937564195</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>
@@ -2454,7 +2454,7 @@
         </is>
       </c>
       <c r="AL8" s="13">
-        <f>IF(X8="","",IF(AN8="Received",0,X8-IF(AJ8&lt;&gt;"",AJ8,0)))</f>
+        <f>IF(X8="","",IF(OR(AN8="Received",AK8="Cleared"),0,X8-IF(AJ8&lt;&gt;"",AJ8,0)))</f>
         <v/>
       </c>
       <c r="AM8" s="13" t="n">
@@ -2530,7 +2530,7 @@
       <c r="AJ9" s="13" t="n"/>
       <c r="AK9" s="11" t="n"/>
       <c r="AL9" s="13">
-        <f>IF(X9="","",IF(AN9="Received",0,X9-IF(AJ9&lt;&gt;"",AJ9,0)))</f>
+        <f>IF(X9="","",IF(OR(AN9="Received",AK9="Cleared"),0,X9-IF(AJ9&lt;&gt;"",AJ9,0)))</f>
         <v/>
       </c>
       <c r="AM9" s="13" t="n"/>
@@ -2594,7 +2594,7 @@
       <c r="AJ10" s="13" t="n"/>
       <c r="AK10" s="11" t="n"/>
       <c r="AL10" s="13">
-        <f>IF(X10="","",IF(AN10="Received",0,X10-IF(AJ10&lt;&gt;"",AJ10,0)))</f>
+        <f>IF(X10="","",IF(OR(AN10="Received",AK10="Cleared"),0,X10-IF(AJ10&lt;&gt;"",AJ10,0)))</f>
         <v/>
       </c>
       <c r="AM10" s="13" t="n"/>
@@ -2658,7 +2658,7 @@
       <c r="AJ11" s="13" t="n"/>
       <c r="AK11" s="11" t="n"/>
       <c r="AL11" s="13">
-        <f>IF(X11="","",IF(AN11="Received",0,X11-IF(AJ11&lt;&gt;"",AJ11,0)))</f>
+        <f>IF(X11="","",IF(OR(AN11="Received",AK11="Cleared"),0,X11-IF(AJ11&lt;&gt;"",AJ11,0)))</f>
         <v/>
       </c>
       <c r="AM11" s="13" t="n"/>
@@ -2722,7 +2722,7 @@
       <c r="AJ12" s="13" t="n"/>
       <c r="AK12" s="11" t="n"/>
       <c r="AL12" s="13">
-        <f>IF(X12="","",IF(AN12="Received",0,X12-IF(AJ12&lt;&gt;"",AJ12,0)))</f>
+        <f>IF(X12="","",IF(OR(AN12="Received",AK12="Cleared"),0,X12-IF(AJ12&lt;&gt;"",AJ12,0)))</f>
         <v/>
       </c>
       <c r="AM12" s="13" t="n"/>
@@ -2786,7 +2786,7 @@
       <c r="AJ13" s="13" t="n"/>
       <c r="AK13" s="11" t="n"/>
       <c r="AL13" s="13">
-        <f>IF(X13="","",IF(AN13="Received",0,X13-IF(AJ13&lt;&gt;"",AJ13,0)))</f>
+        <f>IF(X13="","",IF(OR(AN13="Received",AK13="Cleared"),0,X13-IF(AJ13&lt;&gt;"",AJ13,0)))</f>
         <v/>
       </c>
       <c r="AM13" s="13" t="n"/>
@@ -2850,7 +2850,7 @@
       <c r="AJ14" s="13" t="n"/>
       <c r="AK14" s="11" t="n"/>
       <c r="AL14" s="13">
-        <f>IF(X14="","",IF(AN14="Received",0,X14-IF(AJ14&lt;&gt;"",AJ14,0)))</f>
+        <f>IF(X14="","",IF(OR(AN14="Received",AK14="Cleared"),0,X14-IF(AJ14&lt;&gt;"",AJ14,0)))</f>
         <v/>
       </c>
       <c r="AM14" s="13" t="n"/>
@@ -2914,7 +2914,7 @@
       <c r="AJ15" s="13" t="n"/>
       <c r="AK15" s="11" t="n"/>
       <c r="AL15" s="13">
-        <f>IF(X15="","",IF(AN15="Received",0,X15-IF(AJ15&lt;&gt;"",AJ15,0)))</f>
+        <f>IF(X15="","",IF(OR(AN15="Received",AK15="Cleared"),0,X15-IF(AJ15&lt;&gt;"",AJ15,0)))</f>
         <v/>
       </c>
       <c r="AM15" s="13" t="n"/>
@@ -2978,7 +2978,7 @@
       <c r="AJ16" s="13" t="n"/>
       <c r="AK16" s="11" t="n"/>
       <c r="AL16" s="13">
-        <f>IF(X16="","",IF(AN16="Received",0,X16-IF(AJ16&lt;&gt;"",AJ16,0)))</f>
+        <f>IF(X16="","",IF(OR(AN16="Received",AK16="Cleared"),0,X16-IF(AJ16&lt;&gt;"",AJ16,0)))</f>
         <v/>
       </c>
       <c r="AM16" s="13" t="n"/>
@@ -3042,7 +3042,7 @@
       <c r="AJ17" s="13" t="n"/>
       <c r="AK17" s="11" t="n"/>
       <c r="AL17" s="13">
-        <f>IF(X17="","",IF(AN17="Received",0,X17-IF(AJ17&lt;&gt;"",AJ17,0)))</f>
+        <f>IF(X17="","",IF(OR(AN17="Received",AK17="Cleared"),0,X17-IF(AJ17&lt;&gt;"",AJ17,0)))</f>
         <v/>
       </c>
       <c r="AM17" s="13" t="n"/>
@@ -3106,7 +3106,7 @@
       <c r="AJ18" s="13" t="n"/>
       <c r="AK18" s="11" t="n"/>
       <c r="AL18" s="13">
-        <f>IF(X18="","",IF(AN18="Received",0,X18-IF(AJ18&lt;&gt;"",AJ18,0)))</f>
+        <f>IF(X18="","",IF(OR(AN18="Received",AK18="Cleared"),0,X18-IF(AJ18&lt;&gt;"",AJ18,0)))</f>
         <v/>
       </c>
       <c r="AM18" s="13" t="n"/>
@@ -3170,7 +3170,7 @@
       <c r="AJ19" s="13" t="n"/>
       <c r="AK19" s="11" t="n"/>
       <c r="AL19" s="13">
-        <f>IF(X19="","",IF(AN19="Received",0,X19-IF(AJ19&lt;&gt;"",AJ19,0)))</f>
+        <f>IF(X19="","",IF(OR(AN19="Received",AK19="Cleared"),0,X19-IF(AJ19&lt;&gt;"",AJ19,0)))</f>
         <v/>
       </c>
       <c r="AM19" s="13" t="n"/>
@@ -3234,7 +3234,7 @@
       <c r="AJ20" s="13" t="n"/>
       <c r="AK20" s="11" t="n"/>
       <c r="AL20" s="13">
-        <f>IF(X20="","",IF(AN20="Received",0,X20-IF(AJ20&lt;&gt;"",AJ20,0)))</f>
+        <f>IF(X20="","",IF(OR(AN20="Received",AK20="Cleared"),0,X20-IF(AJ20&lt;&gt;"",AJ20,0)))</f>
         <v/>
       </c>
       <c r="AM20" s="13" t="n"/>
@@ -3298,7 +3298,7 @@
       <c r="AJ21" s="13" t="n"/>
       <c r="AK21" s="11" t="n"/>
       <c r="AL21" s="13">
-        <f>IF(X21="","",IF(AN21="Received",0,X21-IF(AJ21&lt;&gt;"",AJ21,0)))</f>
+        <f>IF(X21="","",IF(OR(AN21="Received",AK21="Cleared"),0,X21-IF(AJ21&lt;&gt;"",AJ21,0)))</f>
         <v/>
       </c>
       <c r="AM21" s="13" t="n"/>
@@ -3362,7 +3362,7 @@
       <c r="AJ22" s="13" t="n"/>
       <c r="AK22" s="11" t="n"/>
       <c r="AL22" s="13">
-        <f>IF(X22="","",IF(AN22="Received",0,X22-IF(AJ22&lt;&gt;"",AJ22,0)))</f>
+        <f>IF(X22="","",IF(OR(AN22="Received",AK22="Cleared"),0,X22-IF(AJ22&lt;&gt;"",AJ22,0)))</f>
         <v/>
       </c>
       <c r="AM22" s="13" t="n"/>
@@ -3426,7 +3426,7 @@
       <c r="AJ23" s="13" t="n"/>
       <c r="AK23" s="11" t="n"/>
       <c r="AL23" s="13">
-        <f>IF(X23="","",IF(AN23="Received",0,X23-IF(AJ23&lt;&gt;"",AJ23,0)))</f>
+        <f>IF(X23="","",IF(OR(AN23="Received",AK23="Cleared"),0,X23-IF(AJ23&lt;&gt;"",AJ23,0)))</f>
         <v/>
       </c>
       <c r="AM23" s="13" t="n"/>
@@ -3490,7 +3490,7 @@
       <c r="AJ24" s="13" t="n"/>
       <c r="AK24" s="11" t="n"/>
       <c r="AL24" s="13">
-        <f>IF(X24="","",IF(AN24="Received",0,X24-IF(AJ24&lt;&gt;"",AJ24,0)))</f>
+        <f>IF(X24="","",IF(OR(AN24="Received",AK24="Cleared"),0,X24-IF(AJ24&lt;&gt;"",AJ24,0)))</f>
         <v/>
       </c>
       <c r="AM24" s="13" t="n"/>
@@ -3554,7 +3554,7 @@
       <c r="AJ25" s="13" t="n"/>
       <c r="AK25" s="11" t="n"/>
       <c r="AL25" s="13">
-        <f>IF(X25="","",IF(AN25="Received",0,X25-IF(AJ25&lt;&gt;"",AJ25,0)))</f>
+        <f>IF(X25="","",IF(OR(AN25="Received",AK25="Cleared"),0,X25-IF(AJ25&lt;&gt;"",AJ25,0)))</f>
         <v/>
       </c>
       <c r="AM25" s="13" t="n"/>
@@ -3618,7 +3618,7 @@
       <c r="AJ26" s="13" t="n"/>
       <c r="AK26" s="11" t="n"/>
       <c r="AL26" s="13">
-        <f>IF(X26="","",IF(AN26="Received",0,X26-IF(AJ26&lt;&gt;"",AJ26,0)))</f>
+        <f>IF(X26="","",IF(OR(AN26="Received",AK26="Cleared"),0,X26-IF(AJ26&lt;&gt;"",AJ26,0)))</f>
         <v/>
       </c>
       <c r="AM26" s="13" t="n"/>
@@ -3682,7 +3682,7 @@
       <c r="AJ27" s="13" t="n"/>
       <c r="AK27" s="11" t="n"/>
       <c r="AL27" s="13">
-        <f>IF(X27="","",IF(AN27="Received",0,X27-IF(AJ27&lt;&gt;"",AJ27,0)))</f>
+        <f>IF(X27="","",IF(OR(AN27="Received",AK27="Cleared"),0,X27-IF(AJ27&lt;&gt;"",AJ27,0)))</f>
         <v/>
       </c>
       <c r="AM27" s="13" t="n"/>
@@ -3746,7 +3746,7 @@
       <c r="AJ28" s="13" t="n"/>
       <c r="AK28" s="11" t="n"/>
       <c r="AL28" s="13">
-        <f>IF(X28="","",IF(AN28="Received",0,X28-IF(AJ28&lt;&gt;"",AJ28,0)))</f>
+        <f>IF(X28="","",IF(OR(AN28="Received",AK28="Cleared"),0,X28-IF(AJ28&lt;&gt;"",AJ28,0)))</f>
         <v/>
       </c>
       <c r="AM28" s="13" t="n"/>
@@ -3810,7 +3810,7 @@
       <c r="AJ29" s="13" t="n"/>
       <c r="AK29" s="11" t="n"/>
       <c r="AL29" s="13">
-        <f>IF(X29="","",IF(AN29="Received",0,X29-IF(AJ29&lt;&gt;"",AJ29,0)))</f>
+        <f>IF(X29="","",IF(OR(AN29="Received",AK29="Cleared"),0,X29-IF(AJ29&lt;&gt;"",AJ29,0)))</f>
         <v/>
       </c>
       <c r="AM29" s="13" t="n"/>
@@ -3874,7 +3874,7 @@
       <c r="AJ30" s="13" t="n"/>
       <c r="AK30" s="11" t="n"/>
       <c r="AL30" s="13">
-        <f>IF(X30="","",IF(AN30="Received",0,X30-IF(AJ30&lt;&gt;"",AJ30,0)))</f>
+        <f>IF(X30="","",IF(OR(AN30="Received",AK30="Cleared"),0,X30-IF(AJ30&lt;&gt;"",AJ30,0)))</f>
         <v/>
       </c>
       <c r="AM30" s="13" t="n"/>
@@ -3938,7 +3938,7 @@
       <c r="AJ31" s="13" t="n"/>
       <c r="AK31" s="11" t="n"/>
       <c r="AL31" s="13">
-        <f>IF(X31="","",IF(AN31="Received",0,X31-IF(AJ31&lt;&gt;"",AJ31,0)))</f>
+        <f>IF(X31="","",IF(OR(AN31="Received",AK31="Cleared"),0,X31-IF(AJ31&lt;&gt;"",AJ31,0)))</f>
         <v/>
       </c>
       <c r="AM31" s="13" t="n"/>
@@ -4002,7 +4002,7 @@
       <c r="AJ32" s="13" t="n"/>
       <c r="AK32" s="11" t="n"/>
       <c r="AL32" s="13">
-        <f>IF(X32="","",IF(AN32="Received",0,X32-IF(AJ32&lt;&gt;"",AJ32,0)))</f>
+        <f>IF(X32="","",IF(OR(AN32="Received",AK32="Cleared"),0,X32-IF(AJ32&lt;&gt;"",AJ32,0)))</f>
         <v/>
       </c>
       <c r="AM32" s="13" t="n"/>
@@ -4066,7 +4066,7 @@
       <c r="AJ33" s="13" t="n"/>
       <c r="AK33" s="11" t="n"/>
       <c r="AL33" s="13">
-        <f>IF(X33="","",IF(AN33="Received",0,X33-IF(AJ33&lt;&gt;"",AJ33,0)))</f>
+        <f>IF(X33="","",IF(OR(AN33="Received",AK33="Cleared"),0,X33-IF(AJ33&lt;&gt;"",AJ33,0)))</f>
         <v/>
       </c>
       <c r="AM33" s="13" t="n"/>
@@ -4130,7 +4130,7 @@
       <c r="AJ34" s="13" t="n"/>
       <c r="AK34" s="11" t="n"/>
       <c r="AL34" s="13">
-        <f>IF(X34="","",IF(AN34="Received",0,X34-IF(AJ34&lt;&gt;"",AJ34,0)))</f>
+        <f>IF(X34="","",IF(OR(AN34="Received",AK34="Cleared"),0,X34-IF(AJ34&lt;&gt;"",AJ34,0)))</f>
         <v/>
       </c>
       <c r="AM34" s="13" t="n"/>
@@ -4194,7 +4194,7 @@
       <c r="AJ35" s="13" t="n"/>
       <c r="AK35" s="11" t="n"/>
       <c r="AL35" s="13">
-        <f>IF(X35="","",IF(AN35="Received",0,X35-IF(AJ35&lt;&gt;"",AJ35,0)))</f>
+        <f>IF(X35="","",IF(OR(AN35="Received",AK35="Cleared"),0,X35-IF(AJ35&lt;&gt;"",AJ35,0)))</f>
         <v/>
       </c>
       <c r="AM35" s="13" t="n"/>
@@ -4258,7 +4258,7 @@
       <c r="AJ36" s="13" t="n"/>
       <c r="AK36" s="11" t="n"/>
       <c r="AL36" s="13">
-        <f>IF(X36="","",IF(AN36="Received",0,X36-IF(AJ36&lt;&gt;"",AJ36,0)))</f>
+        <f>IF(X36="","",IF(OR(AN36="Received",AK36="Cleared"),0,X36-IF(AJ36&lt;&gt;"",AJ36,0)))</f>
         <v/>
       </c>
       <c r="AM36" s="13" t="n"/>
@@ -4322,7 +4322,7 @@
       <c r="AJ37" s="13" t="n"/>
       <c r="AK37" s="11" t="n"/>
       <c r="AL37" s="13">
-        <f>IF(X37="","",IF(AN37="Received",0,X37-IF(AJ37&lt;&gt;"",AJ37,0)))</f>
+        <f>IF(X37="","",IF(OR(AN37="Received",AK37="Cleared"),0,X37-IF(AJ37&lt;&gt;"",AJ37,0)))</f>
         <v/>
       </c>
       <c r="AM37" s="13" t="n"/>
@@ -4386,7 +4386,7 @@
       <c r="AJ38" s="13" t="n"/>
       <c r="AK38" s="11" t="n"/>
       <c r="AL38" s="13">
-        <f>IF(X38="","",IF(AN38="Received",0,X38-IF(AJ38&lt;&gt;"",AJ38,0)))</f>
+        <f>IF(X38="","",IF(OR(AN38="Received",AK38="Cleared"),0,X38-IF(AJ38&lt;&gt;"",AJ38,0)))</f>
         <v/>
       </c>
       <c r="AM38" s="13" t="n"/>
@@ -4450,7 +4450,7 @@
       <c r="AJ39" s="13" t="n"/>
       <c r="AK39" s="11" t="n"/>
       <c r="AL39" s="13">
-        <f>IF(X39="","",IF(AN39="Received",0,X39-IF(AJ39&lt;&gt;"",AJ39,0)))</f>
+        <f>IF(X39="","",IF(OR(AN39="Received",AK39="Cleared"),0,X39-IF(AJ39&lt;&gt;"",AJ39,0)))</f>
         <v/>
       </c>
       <c r="AM39" s="13" t="n"/>
@@ -4514,7 +4514,7 @@
       <c r="AJ40" s="13" t="n"/>
       <c r="AK40" s="11" t="n"/>
       <c r="AL40" s="13">
-        <f>IF(X40="","",IF(AN40="Received",0,X40-IF(AJ40&lt;&gt;"",AJ40,0)))</f>
+        <f>IF(X40="","",IF(OR(AN40="Received",AK40="Cleared"),0,X40-IF(AJ40&lt;&gt;"",AJ40,0)))</f>
         <v/>
       </c>
       <c r="AM40" s="13" t="n"/>
@@ -4578,7 +4578,7 @@
       <c r="AJ41" s="13" t="n"/>
       <c r="AK41" s="11" t="n"/>
       <c r="AL41" s="13">
-        <f>IF(X41="","",IF(AN41="Received",0,X41-IF(AJ41&lt;&gt;"",AJ41,0)))</f>
+        <f>IF(X41="","",IF(OR(AN41="Received",AK41="Cleared"),0,X41-IF(AJ41&lt;&gt;"",AJ41,0)))</f>
         <v/>
       </c>
       <c r="AM41" s="13" t="n"/>
@@ -4642,7 +4642,7 @@
       <c r="AJ42" s="13" t="n"/>
       <c r="AK42" s="11" t="n"/>
       <c r="AL42" s="13">
-        <f>IF(X42="","",IF(AN42="Received",0,X42-IF(AJ42&lt;&gt;"",AJ42,0)))</f>
+        <f>IF(X42="","",IF(OR(AN42="Received",AK42="Cleared"),0,X42-IF(AJ42&lt;&gt;"",AJ42,0)))</f>
         <v/>
       </c>
       <c r="AM42" s="13" t="n"/>
@@ -4706,7 +4706,7 @@
       <c r="AJ43" s="13" t="n"/>
       <c r="AK43" s="11" t="n"/>
       <c r="AL43" s="13">
-        <f>IF(X43="","",IF(AN43="Received",0,X43-IF(AJ43&lt;&gt;"",AJ43,0)))</f>
+        <f>IF(X43="","",IF(OR(AN43="Received",AK43="Cleared"),0,X43-IF(AJ43&lt;&gt;"",AJ43,0)))</f>
         <v/>
       </c>
       <c r="AM43" s="13" t="n"/>
@@ -4770,7 +4770,7 @@
       <c r="AJ44" s="13" t="n"/>
       <c r="AK44" s="11" t="n"/>
       <c r="AL44" s="13">
-        <f>IF(X44="","",IF(AN44="Received",0,X44-IF(AJ44&lt;&gt;"",AJ44,0)))</f>
+        <f>IF(X44="","",IF(OR(AN44="Received",AK44="Cleared"),0,X44-IF(AJ44&lt;&gt;"",AJ44,0)))</f>
         <v/>
       </c>
       <c r="AM44" s="13" t="n"/>
@@ -4834,7 +4834,7 @@
       <c r="AJ45" s="13" t="n"/>
       <c r="AK45" s="11" t="n"/>
       <c r="AL45" s="13">
-        <f>IF(X45="","",IF(AN45="Received",0,X45-IF(AJ45&lt;&gt;"",AJ45,0)))</f>
+        <f>IF(X45="","",IF(OR(AN45="Received",AK45="Cleared"),0,X45-IF(AJ45&lt;&gt;"",AJ45,0)))</f>
         <v/>
       </c>
       <c r="AM45" s="13" t="n"/>
@@ -4898,7 +4898,7 @@
       <c r="AJ46" s="13" t="n"/>
       <c r="AK46" s="11" t="n"/>
       <c r="AL46" s="13">
-        <f>IF(X46="","",IF(AN46="Received",0,X46-IF(AJ46&lt;&gt;"",AJ46,0)))</f>
+        <f>IF(X46="","",IF(OR(AN46="Received",AK46="Cleared"),0,X46-IF(AJ46&lt;&gt;"",AJ46,0)))</f>
         <v/>
       </c>
       <c r="AM46" s="13" t="n"/>
@@ -4962,7 +4962,7 @@
       <c r="AJ47" s="13" t="n"/>
       <c r="AK47" s="11" t="n"/>
       <c r="AL47" s="13">
-        <f>IF(X47="","",IF(AN47="Received",0,X47-IF(AJ47&lt;&gt;"",AJ47,0)))</f>
+        <f>IF(X47="","",IF(OR(AN47="Received",AK47="Cleared"),0,X47-IF(AJ47&lt;&gt;"",AJ47,0)))</f>
         <v/>
       </c>
       <c r="AM47" s="13" t="n"/>
@@ -5026,7 +5026,7 @@
       <c r="AJ48" s="13" t="n"/>
       <c r="AK48" s="11" t="n"/>
       <c r="AL48" s="13">
-        <f>IF(X48="","",IF(AN48="Received",0,X48-IF(AJ48&lt;&gt;"",AJ48,0)))</f>
+        <f>IF(X48="","",IF(OR(AN48="Received",AK48="Cleared"),0,X48-IF(AJ48&lt;&gt;"",AJ48,0)))</f>
         <v/>
       </c>
       <c r="AM48" s="13" t="n"/>
@@ -5090,7 +5090,7 @@
       <c r="AJ49" s="13" t="n"/>
       <c r="AK49" s="11" t="n"/>
       <c r="AL49" s="13">
-        <f>IF(X49="","",IF(AN49="Received",0,X49-IF(AJ49&lt;&gt;"",AJ49,0)))</f>
+        <f>IF(X49="","",IF(OR(AN49="Received",AK49="Cleared"),0,X49-IF(AJ49&lt;&gt;"",AJ49,0)))</f>
         <v/>
       </c>
       <c r="AM49" s="13" t="n"/>
@@ -5154,7 +5154,7 @@
       <c r="AJ50" s="13" t="n"/>
       <c r="AK50" s="11" t="n"/>
       <c r="AL50" s="13">
-        <f>IF(X50="","",IF(AN50="Received",0,X50-IF(AJ50&lt;&gt;"",AJ50,0)))</f>
+        <f>IF(X50="","",IF(OR(AN50="Received",AK50="Cleared"),0,X50-IF(AJ50&lt;&gt;"",AJ50,0)))</f>
         <v/>
       </c>
       <c r="AM50" s="13" t="n"/>
@@ -5218,7 +5218,7 @@
       <c r="AJ51" s="13" t="n"/>
       <c r="AK51" s="11" t="n"/>
       <c r="AL51" s="13">
-        <f>IF(X51="","",IF(AN51="Received",0,X51-IF(AJ51&lt;&gt;"",AJ51,0)))</f>
+        <f>IF(X51="","",IF(OR(AN51="Received",AK51="Cleared"),0,X51-IF(AJ51&lt;&gt;"",AJ51,0)))</f>
         <v/>
       </c>
       <c r="AM51" s="13" t="n"/>
@@ -5282,7 +5282,7 @@
       <c r="AJ52" s="13" t="n"/>
       <c r="AK52" s="11" t="n"/>
       <c r="AL52" s="13">
-        <f>IF(X52="","",IF(AN52="Received",0,X52-IF(AJ52&lt;&gt;"",AJ52,0)))</f>
+        <f>IF(X52="","",IF(OR(AN52="Received",AK52="Cleared"),0,X52-IF(AJ52&lt;&gt;"",AJ52,0)))</f>
         <v/>
       </c>
       <c r="AM52" s="13" t="n"/>
@@ -5346,7 +5346,7 @@
       <c r="AJ53" s="13" t="n"/>
       <c r="AK53" s="11" t="n"/>
       <c r="AL53" s="13">
-        <f>IF(X53="","",IF(AN53="Received",0,X53-IF(AJ53&lt;&gt;"",AJ53,0)))</f>
+        <f>IF(X53="","",IF(OR(AN53="Received",AK53="Cleared"),0,X53-IF(AJ53&lt;&gt;"",AJ53,0)))</f>
         <v/>
       </c>
       <c r="AM53" s="13" t="n"/>
@@ -5410,7 +5410,7 @@
       <c r="AJ54" s="13" t="n"/>
       <c r="AK54" s="11" t="n"/>
       <c r="AL54" s="13">
-        <f>IF(X54="","",IF(AN54="Received",0,X54-IF(AJ54&lt;&gt;"",AJ54,0)))</f>
+        <f>IF(X54="","",IF(OR(AN54="Received",AK54="Cleared"),0,X54-IF(AJ54&lt;&gt;"",AJ54,0)))</f>
         <v/>
       </c>
       <c r="AM54" s="13" t="n"/>
@@ -5474,7 +5474,7 @@
       <c r="AJ55" s="13" t="n"/>
       <c r="AK55" s="11" t="n"/>
       <c r="AL55" s="13">
-        <f>IF(X55="","",IF(AN55="Received",0,X55-IF(AJ55&lt;&gt;"",AJ55,0)))</f>
+        <f>IF(X55="","",IF(OR(AN55="Received",AK55="Cleared"),0,X55-IF(AJ55&lt;&gt;"",AJ55,0)))</f>
         <v/>
       </c>
       <c r="AM55" s="13" t="n"/>
@@ -5538,7 +5538,7 @@
       <c r="AJ56" s="13" t="n"/>
       <c r="AK56" s="11" t="n"/>
       <c r="AL56" s="13">
-        <f>IF(X56="","",IF(AN56="Received",0,X56-IF(AJ56&lt;&gt;"",AJ56,0)))</f>
+        <f>IF(X56="","",IF(OR(AN56="Received",AK56="Cleared"),0,X56-IF(AJ56&lt;&gt;"",AJ56,0)))</f>
         <v/>
       </c>
       <c r="AM56" s="13" t="n"/>
@@ -5602,7 +5602,7 @@
       <c r="AJ57" s="13" t="n"/>
       <c r="AK57" s="11" t="n"/>
       <c r="AL57" s="13">
-        <f>IF(X57="","",IF(AN57="Received",0,X57-IF(AJ57&lt;&gt;"",AJ57,0)))</f>
+        <f>IF(X57="","",IF(OR(AN57="Received",AK57="Cleared"),0,X57-IF(AJ57&lt;&gt;"",AJ57,0)))</f>
         <v/>
       </c>
       <c r="AM57" s="13" t="n"/>
@@ -5666,7 +5666,7 @@
       <c r="AJ58" s="13" t="n"/>
       <c r="AK58" s="11" t="n"/>
       <c r="AL58" s="13">
-        <f>IF(X58="","",IF(AN58="Received",0,X58-IF(AJ58&lt;&gt;"",AJ58,0)))</f>
+        <f>IF(X58="","",IF(OR(AN58="Received",AK58="Cleared"),0,X58-IF(AJ58&lt;&gt;"",AJ58,0)))</f>
         <v/>
       </c>
       <c r="AM58" s="13" t="n"/>
@@ -5730,7 +5730,7 @@
       <c r="AJ59" s="13" t="n"/>
       <c r="AK59" s="11" t="n"/>
       <c r="AL59" s="13">
-        <f>IF(X59="","",IF(AN59="Received",0,X59-IF(AJ59&lt;&gt;"",AJ59,0)))</f>
+        <f>IF(X59="","",IF(OR(AN59="Received",AK59="Cleared"),0,X59-IF(AJ59&lt;&gt;"",AJ59,0)))</f>
         <v/>
       </c>
       <c r="AM59" s="13" t="n"/>
@@ -5794,7 +5794,7 @@
       <c r="AJ60" s="13" t="n"/>
       <c r="AK60" s="11" t="n"/>
       <c r="AL60" s="13">
-        <f>IF(X60="","",IF(AN60="Received",0,X60-IF(AJ60&lt;&gt;"",AJ60,0)))</f>
+        <f>IF(X60="","",IF(OR(AN60="Received",AK60="Cleared"),0,X60-IF(AJ60&lt;&gt;"",AJ60,0)))</f>
         <v/>
       </c>
       <c r="AM60" s="13" t="n"/>
@@ -5858,7 +5858,7 @@
       <c r="AJ61" s="13" t="n"/>
       <c r="AK61" s="11" t="n"/>
       <c r="AL61" s="13">
-        <f>IF(X61="","",IF(AN61="Received",0,X61-IF(AJ61&lt;&gt;"",AJ61,0)))</f>
+        <f>IF(X61="","",IF(OR(AN61="Received",AK61="Cleared"),0,X61-IF(AJ61&lt;&gt;"",AJ61,0)))</f>
         <v/>
       </c>
       <c r="AM61" s="13" t="n"/>
@@ -5922,7 +5922,7 @@
       <c r="AJ62" s="13" t="n"/>
       <c r="AK62" s="11" t="n"/>
       <c r="AL62" s="13">
-        <f>IF(X62="","",IF(AN62="Received",0,X62-IF(AJ62&lt;&gt;"",AJ62,0)))</f>
+        <f>IF(X62="","",IF(OR(AN62="Received",AK62="Cleared"),0,X62-IF(AJ62&lt;&gt;"",AJ62,0)))</f>
         <v/>
       </c>
       <c r="AM62" s="13" t="n"/>
@@ -5986,7 +5986,7 @@
       <c r="AJ63" s="13" t="n"/>
       <c r="AK63" s="11" t="n"/>
       <c r="AL63" s="13">
-        <f>IF(X63="","",IF(AN63="Received",0,X63-IF(AJ63&lt;&gt;"",AJ63,0)))</f>
+        <f>IF(X63="","",IF(OR(AN63="Received",AK63="Cleared"),0,X63-IF(AJ63&lt;&gt;"",AJ63,0)))</f>
         <v/>
       </c>
       <c r="AM63" s="13" t="n"/>
@@ -6050,7 +6050,7 @@
       <c r="AJ64" s="13" t="n"/>
       <c r="AK64" s="11" t="n"/>
       <c r="AL64" s="13">
-        <f>IF(X64="","",IF(AN64="Received",0,X64-IF(AJ64&lt;&gt;"",AJ64,0)))</f>
+        <f>IF(X64="","",IF(OR(AN64="Received",AK64="Cleared"),0,X64-IF(AJ64&lt;&gt;"",AJ64,0)))</f>
         <v/>
       </c>
       <c r="AM64" s="13" t="n"/>
@@ -6114,7 +6114,7 @@
       <c r="AJ65" s="13" t="n"/>
       <c r="AK65" s="11" t="n"/>
       <c r="AL65" s="13">
-        <f>IF(X65="","",IF(AN65="Received",0,X65-IF(AJ65&lt;&gt;"",AJ65,0)))</f>
+        <f>IF(X65="","",IF(OR(AN65="Received",AK65="Cleared"),0,X65-IF(AJ65&lt;&gt;"",AJ65,0)))</f>
         <v/>
       </c>
       <c r="AM65" s="13" t="n"/>
@@ -6178,7 +6178,7 @@
       <c r="AJ66" s="13" t="n"/>
       <c r="AK66" s="11" t="n"/>
       <c r="AL66" s="13">
-        <f>IF(X66="","",IF(AN66="Received",0,X66-IF(AJ66&lt;&gt;"",AJ66,0)))</f>
+        <f>IF(X66="","",IF(OR(AN66="Received",AK66="Cleared"),0,X66-IF(AJ66&lt;&gt;"",AJ66,0)))</f>
         <v/>
       </c>
       <c r="AM66" s="13" t="n"/>
@@ -6242,7 +6242,7 @@
       <c r="AJ67" s="13" t="n"/>
       <c r="AK67" s="11" t="n"/>
       <c r="AL67" s="13">
-        <f>IF(X67="","",IF(AN67="Received",0,X67-IF(AJ67&lt;&gt;"",AJ67,0)))</f>
+        <f>IF(X67="","",IF(OR(AN67="Received",AK67="Cleared"),0,X67-IF(AJ67&lt;&gt;"",AJ67,0)))</f>
         <v/>
       </c>
       <c r="AM67" s="13" t="n"/>
@@ -6306,7 +6306,7 @@
       <c r="AJ68" s="13" t="n"/>
       <c r="AK68" s="11" t="n"/>
       <c r="AL68" s="13">
-        <f>IF(X68="","",IF(AN68="Received",0,X68-IF(AJ68&lt;&gt;"",AJ68,0)))</f>
+        <f>IF(X68="","",IF(OR(AN68="Received",AK68="Cleared"),0,X68-IF(AJ68&lt;&gt;"",AJ68,0)))</f>
         <v/>
       </c>
       <c r="AM68" s="13" t="n"/>
@@ -6370,7 +6370,7 @@
       <c r="AJ69" s="13" t="n"/>
       <c r="AK69" s="11" t="n"/>
       <c r="AL69" s="13">
-        <f>IF(X69="","",IF(AN69="Received",0,X69-IF(AJ69&lt;&gt;"",AJ69,0)))</f>
+        <f>IF(X69="","",IF(OR(AN69="Received",AK69="Cleared"),0,X69-IF(AJ69&lt;&gt;"",AJ69,0)))</f>
         <v/>
       </c>
       <c r="AM69" s="13" t="n"/>
@@ -6434,7 +6434,7 @@
       <c r="AJ70" s="13" t="n"/>
       <c r="AK70" s="11" t="n"/>
       <c r="AL70" s="13">
-        <f>IF(X70="","",IF(AN70="Received",0,X70-IF(AJ70&lt;&gt;"",AJ70,0)))</f>
+        <f>IF(X70="","",IF(OR(AN70="Received",AK70="Cleared"),0,X70-IF(AJ70&lt;&gt;"",AJ70,0)))</f>
         <v/>
       </c>
       <c r="AM70" s="13" t="n"/>
@@ -6498,7 +6498,7 @@
       <c r="AJ71" s="13" t="n"/>
       <c r="AK71" s="11" t="n"/>
       <c r="AL71" s="13">
-        <f>IF(X71="","",IF(AN71="Received",0,X71-IF(AJ71&lt;&gt;"",AJ71,0)))</f>
+        <f>IF(X71="","",IF(OR(AN71="Received",AK71="Cleared"),0,X71-IF(AJ71&lt;&gt;"",AJ71,0)))</f>
         <v/>
       </c>
       <c r="AM71" s="13" t="n"/>
@@ -6562,7 +6562,7 @@
       <c r="AJ72" s="13" t="n"/>
       <c r="AK72" s="11" t="n"/>
       <c r="AL72" s="13">
-        <f>IF(X72="","",IF(AN72="Received",0,X72-IF(AJ72&lt;&gt;"",AJ72,0)))</f>
+        <f>IF(X72="","",IF(OR(AN72="Received",AK72="Cleared"),0,X72-IF(AJ72&lt;&gt;"",AJ72,0)))</f>
         <v/>
       </c>
       <c r="AM72" s="13" t="n"/>
@@ -6626,7 +6626,7 @@
       <c r="AJ73" s="13" t="n"/>
       <c r="AK73" s="11" t="n"/>
       <c r="AL73" s="13">
-        <f>IF(X73="","",IF(AN73="Received",0,X73-IF(AJ73&lt;&gt;"",AJ73,0)))</f>
+        <f>IF(X73="","",IF(OR(AN73="Received",AK73="Cleared"),0,X73-IF(AJ73&lt;&gt;"",AJ73,0)))</f>
         <v/>
       </c>
       <c r="AM73" s="13" t="n"/>
@@ -6690,7 +6690,7 @@
       <c r="AJ74" s="13" t="n"/>
       <c r="AK74" s="11" t="n"/>
       <c r="AL74" s="13">
-        <f>IF(X74="","",IF(AN74="Received",0,X74-IF(AJ74&lt;&gt;"",AJ74,0)))</f>
+        <f>IF(X74="","",IF(OR(AN74="Received",AK74="Cleared"),0,X74-IF(AJ74&lt;&gt;"",AJ74,0)))</f>
         <v/>
       </c>
       <c r="AM74" s="13" t="n"/>
@@ -6754,7 +6754,7 @@
       <c r="AJ75" s="13" t="n"/>
       <c r="AK75" s="11" t="n"/>
       <c r="AL75" s="13">
-        <f>IF(X75="","",IF(AN75="Received",0,X75-IF(AJ75&lt;&gt;"",AJ75,0)))</f>
+        <f>IF(X75="","",IF(OR(AN75="Received",AK75="Cleared"),0,X75-IF(AJ75&lt;&gt;"",AJ75,0)))</f>
         <v/>
       </c>
       <c r="AM75" s="13" t="n"/>
@@ -6818,7 +6818,7 @@
       <c r="AJ76" s="13" t="n"/>
       <c r="AK76" s="11" t="n"/>
       <c r="AL76" s="13">
-        <f>IF(X76="","",IF(AN76="Received",0,X76-IF(AJ76&lt;&gt;"",AJ76,0)))</f>
+        <f>IF(X76="","",IF(OR(AN76="Received",AK76="Cleared"),0,X76-IF(AJ76&lt;&gt;"",AJ76,0)))</f>
         <v/>
       </c>
       <c r="AM76" s="13" t="n"/>
@@ -6882,7 +6882,7 @@
       <c r="AJ77" s="13" t="n"/>
       <c r="AK77" s="11" t="n"/>
       <c r="AL77" s="13">
-        <f>IF(X77="","",IF(AN77="Received",0,X77-IF(AJ77&lt;&gt;"",AJ77,0)))</f>
+        <f>IF(X77="","",IF(OR(AN77="Received",AK77="Cleared"),0,X77-IF(AJ77&lt;&gt;"",AJ77,0)))</f>
         <v/>
       </c>
       <c r="AM77" s="13" t="n"/>
@@ -6946,7 +6946,7 @@
       <c r="AJ78" s="13" t="n"/>
       <c r="AK78" s="11" t="n"/>
       <c r="AL78" s="13">
-        <f>IF(X78="","",IF(AN78="Received",0,X78-IF(AJ78&lt;&gt;"",AJ78,0)))</f>
+        <f>IF(X78="","",IF(OR(AN78="Received",AK78="Cleared"),0,X78-IF(AJ78&lt;&gt;"",AJ78,0)))</f>
         <v/>
       </c>
       <c r="AM78" s="13" t="n"/>
@@ -7010,7 +7010,7 @@
       <c r="AJ79" s="13" t="n"/>
       <c r="AK79" s="11" t="n"/>
       <c r="AL79" s="13">
-        <f>IF(X79="","",IF(AN79="Received",0,X79-IF(AJ79&lt;&gt;"",AJ79,0)))</f>
+        <f>IF(X79="","",IF(OR(AN79="Received",AK79="Cleared"),0,X79-IF(AJ79&lt;&gt;"",AJ79,0)))</f>
         <v/>
       </c>
       <c r="AM79" s="13" t="n"/>
@@ -7074,7 +7074,7 @@
       <c r="AJ80" s="13" t="n"/>
       <c r="AK80" s="11" t="n"/>
       <c r="AL80" s="13">
-        <f>IF(X80="","",IF(AN80="Received",0,X80-IF(AJ80&lt;&gt;"",AJ80,0)))</f>
+        <f>IF(X80="","",IF(OR(AN80="Received",AK80="Cleared"),0,X80-IF(AJ80&lt;&gt;"",AJ80,0)))</f>
         <v/>
       </c>
       <c r="AM80" s="13" t="n"/>
@@ -7138,7 +7138,7 @@
       <c r="AJ81" s="13" t="n"/>
       <c r="AK81" s="11" t="n"/>
       <c r="AL81" s="13">
-        <f>IF(X81="","",IF(AN81="Received",0,X81-IF(AJ81&lt;&gt;"",AJ81,0)))</f>
+        <f>IF(X81="","",IF(OR(AN81="Received",AK81="Cleared"),0,X81-IF(AJ81&lt;&gt;"",AJ81,0)))</f>
         <v/>
       </c>
       <c r="AM81" s="13" t="n"/>
@@ -7202,7 +7202,7 @@
       <c r="AJ82" s="13" t="n"/>
       <c r="AK82" s="11" t="n"/>
       <c r="AL82" s="13">
-        <f>IF(X82="","",IF(AN82="Received",0,X82-IF(AJ82&lt;&gt;"",AJ82,0)))</f>
+        <f>IF(X82="","",IF(OR(AN82="Received",AK82="Cleared"),0,X82-IF(AJ82&lt;&gt;"",AJ82,0)))</f>
         <v/>
       </c>
       <c r="AM82" s="13" t="n"/>
@@ -7266,7 +7266,7 @@
       <c r="AJ83" s="13" t="n"/>
       <c r="AK83" s="11" t="n"/>
       <c r="AL83" s="13">
-        <f>IF(X83="","",IF(AN83="Received",0,X83-IF(AJ83&lt;&gt;"",AJ83,0)))</f>
+        <f>IF(X83="","",IF(OR(AN83="Received",AK83="Cleared"),0,X83-IF(AJ83&lt;&gt;"",AJ83,0)))</f>
         <v/>
       </c>
       <c r="AM83" s="13" t="n"/>
@@ -7330,7 +7330,7 @@
       <c r="AJ84" s="13" t="n"/>
       <c r="AK84" s="11" t="n"/>
       <c r="AL84" s="13">
-        <f>IF(X84="","",IF(AN84="Received",0,X84-IF(AJ84&lt;&gt;"",AJ84,0)))</f>
+        <f>IF(X84="","",IF(OR(AN84="Received",AK84="Cleared"),0,X84-IF(AJ84&lt;&gt;"",AJ84,0)))</f>
         <v/>
       </c>
       <c r="AM84" s="13" t="n"/>
@@ -7394,7 +7394,7 @@
       <c r="AJ85" s="13" t="n"/>
       <c r="AK85" s="11" t="n"/>
       <c r="AL85" s="13">
-        <f>IF(X85="","",IF(AN85="Received",0,X85-IF(AJ85&lt;&gt;"",AJ85,0)))</f>
+        <f>IF(X85="","",IF(OR(AN85="Received",AK85="Cleared"),0,X85-IF(AJ85&lt;&gt;"",AJ85,0)))</f>
         <v/>
       </c>
       <c r="AM85" s="13" t="n"/>
@@ -7458,7 +7458,7 @@
       <c r="AJ86" s="13" t="n"/>
       <c r="AK86" s="11" t="n"/>
       <c r="AL86" s="13">
-        <f>IF(X86="","",IF(AN86="Received",0,X86-IF(AJ86&lt;&gt;"",AJ86,0)))</f>
+        <f>IF(X86="","",IF(OR(AN86="Received",AK86="Cleared"),0,X86-IF(AJ86&lt;&gt;"",AJ86,0)))</f>
         <v/>
       </c>
       <c r="AM86" s="13" t="n"/>
@@ -7522,7 +7522,7 @@
       <c r="AJ87" s="13" t="n"/>
       <c r="AK87" s="11" t="n"/>
       <c r="AL87" s="13">
-        <f>IF(X87="","",IF(AN87="Received",0,X87-IF(AJ87&lt;&gt;"",AJ87,0)))</f>
+        <f>IF(X87="","",IF(OR(AN87="Received",AK87="Cleared"),0,X87-IF(AJ87&lt;&gt;"",AJ87,0)))</f>
         <v/>
       </c>
       <c r="AM87" s="13" t="n"/>
@@ -7586,7 +7586,7 @@
       <c r="AJ88" s="13" t="n"/>
       <c r="AK88" s="11" t="n"/>
       <c r="AL88" s="13">
-        <f>IF(X88="","",IF(AN88="Received",0,X88-IF(AJ88&lt;&gt;"",AJ88,0)))</f>
+        <f>IF(X88="","",IF(OR(AN88="Received",AK88="Cleared"),0,X88-IF(AJ88&lt;&gt;"",AJ88,0)))</f>
         <v/>
       </c>
       <c r="AM88" s="13" t="n"/>
@@ -7650,7 +7650,7 @@
       <c r="AJ89" s="13" t="n"/>
       <c r="AK89" s="11" t="n"/>
       <c r="AL89" s="13">
-        <f>IF(X89="","",IF(AN89="Received",0,X89-IF(AJ89&lt;&gt;"",AJ89,0)))</f>
+        <f>IF(X89="","",IF(OR(AN89="Received",AK89="Cleared"),0,X89-IF(AJ89&lt;&gt;"",AJ89,0)))</f>
         <v/>
       </c>
       <c r="AM89" s="13" t="n"/>
@@ -7714,7 +7714,7 @@
       <c r="AJ90" s="13" t="n"/>
       <c r="AK90" s="11" t="n"/>
       <c r="AL90" s="13">
-        <f>IF(X90="","",IF(AN90="Received",0,X90-IF(AJ90&lt;&gt;"",AJ90,0)))</f>
+        <f>IF(X90="","",IF(OR(AN90="Received",AK90="Cleared"),0,X90-IF(AJ90&lt;&gt;"",AJ90,0)))</f>
         <v/>
       </c>
       <c r="AM90" s="13" t="n"/>
@@ -7778,7 +7778,7 @@
       <c r="AJ91" s="13" t="n"/>
       <c r="AK91" s="11" t="n"/>
       <c r="AL91" s="13">
-        <f>IF(X91="","",IF(AN91="Received",0,X91-IF(AJ91&lt;&gt;"",AJ91,0)))</f>
+        <f>IF(X91="","",IF(OR(AN91="Received",AK91="Cleared"),0,X91-IF(AJ91&lt;&gt;"",AJ91,0)))</f>
         <v/>
       </c>
       <c r="AM91" s="13" t="n"/>
@@ -7842,7 +7842,7 @@
       <c r="AJ92" s="13" t="n"/>
       <c r="AK92" s="11" t="n"/>
       <c r="AL92" s="13">
-        <f>IF(X92="","",IF(AN92="Received",0,X92-IF(AJ92&lt;&gt;"",AJ92,0)))</f>
+        <f>IF(X92="","",IF(OR(AN92="Received",AK92="Cleared"),0,X92-IF(AJ92&lt;&gt;"",AJ92,0)))</f>
         <v/>
       </c>
       <c r="AM92" s="13" t="n"/>
@@ -7906,7 +7906,7 @@
       <c r="AJ93" s="13" t="n"/>
       <c r="AK93" s="11" t="n"/>
       <c r="AL93" s="13">
-        <f>IF(X93="","",IF(AN93="Received",0,X93-IF(AJ93&lt;&gt;"",AJ93,0)))</f>
+        <f>IF(X93="","",IF(OR(AN93="Received",AK93="Cleared"),0,X93-IF(AJ93&lt;&gt;"",AJ93,0)))</f>
         <v/>
       </c>
       <c r="AM93" s="13" t="n"/>
@@ -7970,7 +7970,7 @@
       <c r="AJ94" s="13" t="n"/>
       <c r="AK94" s="11" t="n"/>
       <c r="AL94" s="13">
-        <f>IF(X94="","",IF(AN94="Received",0,X94-IF(AJ94&lt;&gt;"",AJ94,0)))</f>
+        <f>IF(X94="","",IF(OR(AN94="Received",AK94="Cleared"),0,X94-IF(AJ94&lt;&gt;"",AJ94,0)))</f>
         <v/>
       </c>
       <c r="AM94" s="13" t="n"/>
@@ -8034,7 +8034,7 @@
       <c r="AJ95" s="13" t="n"/>
       <c r="AK95" s="11" t="n"/>
       <c r="AL95" s="13">
-        <f>IF(X95="","",IF(AN95="Received",0,X95-IF(AJ95&lt;&gt;"",AJ95,0)))</f>
+        <f>IF(X95="","",IF(OR(AN95="Received",AK95="Cleared"),0,X95-IF(AJ95&lt;&gt;"",AJ95,0)))</f>
         <v/>
       </c>
       <c r="AM95" s="13" t="n"/>
@@ -8098,7 +8098,7 @@
       <c r="AJ96" s="13" t="n"/>
       <c r="AK96" s="11" t="n"/>
       <c r="AL96" s="13">
-        <f>IF(X96="","",IF(AN96="Received",0,X96-IF(AJ96&lt;&gt;"",AJ96,0)))</f>
+        <f>IF(X96="","",IF(OR(AN96="Received",AK96="Cleared"),0,X96-IF(AJ96&lt;&gt;"",AJ96,0)))</f>
         <v/>
       </c>
       <c r="AM96" s="13" t="n"/>
@@ -8162,7 +8162,7 @@
       <c r="AJ97" s="13" t="n"/>
       <c r="AK97" s="11" t="n"/>
       <c r="AL97" s="13">
-        <f>IF(X97="","",IF(AN97="Received",0,X97-IF(AJ97&lt;&gt;"",AJ97,0)))</f>
+        <f>IF(X97="","",IF(OR(AN97="Received",AK97="Cleared"),0,X97-IF(AJ97&lt;&gt;"",AJ97,0)))</f>
         <v/>
       </c>
       <c r="AM97" s="13" t="n"/>
@@ -8226,7 +8226,7 @@
       <c r="AJ98" s="13" t="n"/>
       <c r="AK98" s="11" t="n"/>
       <c r="AL98" s="13">
-        <f>IF(X98="","",IF(AN98="Received",0,X98-IF(AJ98&lt;&gt;"",AJ98,0)))</f>
+        <f>IF(X98="","",IF(OR(AN98="Received",AK98="Cleared"),0,X98-IF(AJ98&lt;&gt;"",AJ98,0)))</f>
         <v/>
       </c>
       <c r="AM98" s="13" t="n"/>
@@ -8290,7 +8290,7 @@
       <c r="AJ99" s="13" t="n"/>
       <c r="AK99" s="11" t="n"/>
       <c r="AL99" s="13">
-        <f>IF(X99="","",IF(AN99="Received",0,X99-IF(AJ99&lt;&gt;"",AJ99,0)))</f>
+        <f>IF(X99="","",IF(OR(AN99="Received",AK99="Cleared"),0,X99-IF(AJ99&lt;&gt;"",AJ99,0)))</f>
         <v/>
       </c>
       <c r="AM99" s="13" t="n"/>
@@ -8354,7 +8354,7 @@
       <c r="AJ100" s="13" t="n"/>
       <c r="AK100" s="11" t="n"/>
       <c r="AL100" s="13">
-        <f>IF(X100="","",IF(AN100="Received",0,X100-IF(AJ100&lt;&gt;"",AJ100,0)))</f>
+        <f>IF(X100="","",IF(OR(AN100="Received",AK100="Cleared"),0,X100-IF(AJ100&lt;&gt;"",AJ100,0)))</f>
         <v/>
       </c>
       <c r="AM100" s="13" t="n"/>

</xml_diff>

<commit_message>
Fresh regeneration - no date validation on dashboard
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.76937564195</v>
+        <v>46044.77150127743</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1891,7 +1891,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.76937564195</v>
+        <v>46051.77150127743</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.76937564195</v>
+        <v>46051.77150127743</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.76937564195</v>
+        <v>46046.77150127743</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2027,7 +2027,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.76937564195</v>
+        <v>46054.77150127743</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2073,7 +2073,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.76937564195</v>
+        <v>46042.77150127743</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2195,7 +2195,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.76937564195</v>
+        <v>46047.77150127743</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2269,7 +2269,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.76937564195</v>
+        <v>46052.77150127743</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.76937564195</v>
+        <v>46052.77150127743</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2335,7 +2335,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.76937564195</v>
+        <v>46039.77150127743</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2405,7 +2405,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.76937564195</v>
+        <v>46041.77150127743</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.76937564195</v>
+        <v>46041.77150127743</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.76937564195</v>
+        <v>46041.77150127743</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Pre-fill From/To dates so Google Sheets recognizes date format
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -21,10 +21,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="DD-MMM-YYYY HH:MM"/>
     <numFmt numFmtId="165" formatCode="₹#,##0"/>
     <numFmt numFmtId="166" formatCode="DD-MMM-YYYY"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -1809,7 +1810,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.77150127743</v>
+        <v>46044.77315780267</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1891,7 +1892,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.77150127743</v>
+        <v>46051.77315780267</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1921,7 +1922,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.77150127743</v>
+        <v>46051.77315780267</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1957,7 +1958,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.77150127743</v>
+        <v>46046.77315780267</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2027,7 +2028,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.77150127743</v>
+        <v>46054.77315780267</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2073,7 +2074,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.77150127743</v>
+        <v>46042.77315780267</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2195,7 +2196,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.77150127743</v>
+        <v>46047.77315780267</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2269,7 +2270,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.77150127743</v>
+        <v>46052.77315780267</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2299,7 +2300,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.77150127743</v>
+        <v>46052.77315780267</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2335,7 +2336,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.77150127743</v>
+        <v>46039.77315780267</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2405,7 +2406,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.77150127743</v>
+        <v>46041.77315780267</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2435,7 +2436,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.77150127743</v>
+        <v>46041.77315780267</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2443,7 +2444,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.77150127743</v>
+        <v>46041.77315780267</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>
@@ -9809,16 +9810,20 @@
           <t>From Date</t>
         </is>
       </c>
-      <c r="B60" s="36" t="n"/>
+      <c r="B60" s="36" t="n">
+        <v>46039</v>
+      </c>
       <c r="C60" s="35" t="inlineStr">
         <is>
           <t>To Date</t>
         </is>
       </c>
-      <c r="D60" s="36" t="n"/>
+      <c r="D60" s="36" t="n">
+        <v>46050</v>
+      </c>
       <c r="F60" s="37" t="inlineStr">
         <is>
-          <t>← Type date like 17/01/2026 or 17-Jan-2026</t>
+          <t>← Clear and type your dates (e.g. 17/01/2026)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fresh build - no date validation on dashboard, pre-filled dates
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1810,7 +1810,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.77315780267</v>
+        <v>46044.7767419695</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1892,7 +1892,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.77315780267</v>
+        <v>46051.7767419695</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.77315780267</v>
+        <v>46051.7767419695</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1958,7 +1958,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.77315780267</v>
+        <v>46046.7767419695</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2028,7 +2028,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.77315780267</v>
+        <v>46054.7767419695</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.77315780267</v>
+        <v>46042.7767419695</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2196,7 +2196,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.77315780267</v>
+        <v>46047.7767419695</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2270,7 +2270,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.77315780267</v>
+        <v>46052.7767419695</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.77315780267</v>
+        <v>46052.7767419695</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.77315780267</v>
+        <v>46039.7767419695</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2406,7 +2406,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.77315780267</v>
+        <v>46041.7767419695</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.77315780267</v>
+        <v>46041.7767419695</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.77315780267</v>
+        <v>46041.7767419695</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Add Refund Completed to Payment Status dropdown + dashboard tracking
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1405,7 +1405,7 @@
     <row r="11" ht="55" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>GREEN = Confirmed / Payment Received  |  YELLOW = Pending / Advance NIL  |  RED = Cancelled / Payment Pending  |  BLUE = Scheduled  |  PURPLE tint = Completed  |  ORANGE = Refunded</t>
+          <t>GREEN = Confirmed / Payment Received  |  YELLOW = Pending / Advance NIL  |  RED = Cancelled / Payment Pending  |  BLUE = Scheduled  |  PURPLE tint = Completed  |  ORANGE = Refunded / Refund Completed</t>
         </is>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.7767419695</v>
+        <v>46044.78111086666</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1892,7 +1892,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.7767419695</v>
+        <v>46051.78111086666</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.7767419695</v>
+        <v>46051.78111086666</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1939,7 +1939,7 @@
         </is>
       </c>
       <c r="AL4" s="13">
-        <f>IF(X4="","",IF(OR(AN4="Received",AK4="Cleared"),0,X4-IF(AJ4&lt;&gt;"",AJ4,0)))</f>
+        <f>IF(X4="","",IF(OR(AN4="Received",AK4="Cleared",AN4="Refund Completed"),0,X4-IF(AJ4&lt;&gt;"",AJ4,0)))</f>
         <v/>
       </c>
       <c r="AM4" s="13" t="n"/>
@@ -1958,7 +1958,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.7767419695</v>
+        <v>46046.78111086666</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2028,7 +2028,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.7767419695</v>
+        <v>46054.78111086666</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2055,7 +2055,7 @@
       <c r="AJ5" s="13" t="n"/>
       <c r="AK5" s="11" t="n"/>
       <c r="AL5" s="13">
-        <f>IF(X5="","",IF(OR(AN5="Received",AK5="Cleared"),0,X5-IF(AJ5&lt;&gt;"",AJ5,0)))</f>
+        <f>IF(X5="","",IF(OR(AN5="Received",AK5="Cleared",AN5="Refund Completed"),0,X5-IF(AJ5&lt;&gt;"",AJ5,0)))</f>
         <v/>
       </c>
       <c r="AM5" s="13" t="n"/>
@@ -2074,7 +2074,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.7767419695</v>
+        <v>46042.78111086666</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2177,7 +2177,7 @@
       <c r="AJ6" s="13" t="n"/>
       <c r="AK6" s="11" t="n"/>
       <c r="AL6" s="13">
-        <f>IF(X6="","",IF(OR(AN6="Received",AK6="Cleared"),0,X6-IF(AJ6&lt;&gt;"",AJ6,0)))</f>
+        <f>IF(X6="","",IF(OR(AN6="Received",AK6="Cleared",AN6="Refund Completed"),0,X6-IF(AJ6&lt;&gt;"",AJ6,0)))</f>
         <v/>
       </c>
       <c r="AM6" s="13" t="n"/>
@@ -2196,7 +2196,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.7767419695</v>
+        <v>46047.78111086666</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2270,7 +2270,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.7767419695</v>
+        <v>46052.78111086666</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.7767419695</v>
+        <v>46052.78111086666</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="AL7" s="13">
-        <f>IF(X7="","",IF(OR(AN7="Received",AK7="Cleared"),0,X7-IF(AJ7&lt;&gt;"",AJ7,0)))</f>
+        <f>IF(X7="","",IF(OR(AN7="Received",AK7="Cleared",AN7="Refund Completed"),0,X7-IF(AJ7&lt;&gt;"",AJ7,0)))</f>
         <v/>
       </c>
       <c r="AM7" s="13" t="n"/>
@@ -2336,7 +2336,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.7767419695</v>
+        <v>46039.78111086666</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2406,7 +2406,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.7767419695</v>
+        <v>46041.78111086666</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.7767419695</v>
+        <v>46041.78111086666</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.7767419695</v>
+        <v>46041.78111086666</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>
@@ -2455,7 +2455,7 @@
         </is>
       </c>
       <c r="AL8" s="13">
-        <f>IF(X8="","",IF(OR(AN8="Received",AK8="Cleared"),0,X8-IF(AJ8&lt;&gt;"",AJ8,0)))</f>
+        <f>IF(X8="","",IF(OR(AN8="Received",AK8="Cleared",AN8="Refund Completed"),0,X8-IF(AJ8&lt;&gt;"",AJ8,0)))</f>
         <v/>
       </c>
       <c r="AM8" s="13" t="n">
@@ -2531,7 +2531,7 @@
       <c r="AJ9" s="13" t="n"/>
       <c r="AK9" s="11" t="n"/>
       <c r="AL9" s="13">
-        <f>IF(X9="","",IF(OR(AN9="Received",AK9="Cleared"),0,X9-IF(AJ9&lt;&gt;"",AJ9,0)))</f>
+        <f>IF(X9="","",IF(OR(AN9="Received",AK9="Cleared",AN9="Refund Completed"),0,X9-IF(AJ9&lt;&gt;"",AJ9,0)))</f>
         <v/>
       </c>
       <c r="AM9" s="13" t="n"/>
@@ -2595,7 +2595,7 @@
       <c r="AJ10" s="13" t="n"/>
       <c r="AK10" s="11" t="n"/>
       <c r="AL10" s="13">
-        <f>IF(X10="","",IF(OR(AN10="Received",AK10="Cleared"),0,X10-IF(AJ10&lt;&gt;"",AJ10,0)))</f>
+        <f>IF(X10="","",IF(OR(AN10="Received",AK10="Cleared",AN10="Refund Completed"),0,X10-IF(AJ10&lt;&gt;"",AJ10,0)))</f>
         <v/>
       </c>
       <c r="AM10" s="13" t="n"/>
@@ -2659,7 +2659,7 @@
       <c r="AJ11" s="13" t="n"/>
       <c r="AK11" s="11" t="n"/>
       <c r="AL11" s="13">
-        <f>IF(X11="","",IF(OR(AN11="Received",AK11="Cleared"),0,X11-IF(AJ11&lt;&gt;"",AJ11,0)))</f>
+        <f>IF(X11="","",IF(OR(AN11="Received",AK11="Cleared",AN11="Refund Completed"),0,X11-IF(AJ11&lt;&gt;"",AJ11,0)))</f>
         <v/>
       </c>
       <c r="AM11" s="13" t="n"/>
@@ -2723,7 +2723,7 @@
       <c r="AJ12" s="13" t="n"/>
       <c r="AK12" s="11" t="n"/>
       <c r="AL12" s="13">
-        <f>IF(X12="","",IF(OR(AN12="Received",AK12="Cleared"),0,X12-IF(AJ12&lt;&gt;"",AJ12,0)))</f>
+        <f>IF(X12="","",IF(OR(AN12="Received",AK12="Cleared",AN12="Refund Completed"),0,X12-IF(AJ12&lt;&gt;"",AJ12,0)))</f>
         <v/>
       </c>
       <c r="AM12" s="13" t="n"/>
@@ -2787,7 +2787,7 @@
       <c r="AJ13" s="13" t="n"/>
       <c r="AK13" s="11" t="n"/>
       <c r="AL13" s="13">
-        <f>IF(X13="","",IF(OR(AN13="Received",AK13="Cleared"),0,X13-IF(AJ13&lt;&gt;"",AJ13,0)))</f>
+        <f>IF(X13="","",IF(OR(AN13="Received",AK13="Cleared",AN13="Refund Completed"),0,X13-IF(AJ13&lt;&gt;"",AJ13,0)))</f>
         <v/>
       </c>
       <c r="AM13" s="13" t="n"/>
@@ -2851,7 +2851,7 @@
       <c r="AJ14" s="13" t="n"/>
       <c r="AK14" s="11" t="n"/>
       <c r="AL14" s="13">
-        <f>IF(X14="","",IF(OR(AN14="Received",AK14="Cleared"),0,X14-IF(AJ14&lt;&gt;"",AJ14,0)))</f>
+        <f>IF(X14="","",IF(OR(AN14="Received",AK14="Cleared",AN14="Refund Completed"),0,X14-IF(AJ14&lt;&gt;"",AJ14,0)))</f>
         <v/>
       </c>
       <c r="AM14" s="13" t="n"/>
@@ -2915,7 +2915,7 @@
       <c r="AJ15" s="13" t="n"/>
       <c r="AK15" s="11" t="n"/>
       <c r="AL15" s="13">
-        <f>IF(X15="","",IF(OR(AN15="Received",AK15="Cleared"),0,X15-IF(AJ15&lt;&gt;"",AJ15,0)))</f>
+        <f>IF(X15="","",IF(OR(AN15="Received",AK15="Cleared",AN15="Refund Completed"),0,X15-IF(AJ15&lt;&gt;"",AJ15,0)))</f>
         <v/>
       </c>
       <c r="AM15" s="13" t="n"/>
@@ -2979,7 +2979,7 @@
       <c r="AJ16" s="13" t="n"/>
       <c r="AK16" s="11" t="n"/>
       <c r="AL16" s="13">
-        <f>IF(X16="","",IF(OR(AN16="Received",AK16="Cleared"),0,X16-IF(AJ16&lt;&gt;"",AJ16,0)))</f>
+        <f>IF(X16="","",IF(OR(AN16="Received",AK16="Cleared",AN16="Refund Completed"),0,X16-IF(AJ16&lt;&gt;"",AJ16,0)))</f>
         <v/>
       </c>
       <c r="AM16" s="13" t="n"/>
@@ -3043,7 +3043,7 @@
       <c r="AJ17" s="13" t="n"/>
       <c r="AK17" s="11" t="n"/>
       <c r="AL17" s="13">
-        <f>IF(X17="","",IF(OR(AN17="Received",AK17="Cleared"),0,X17-IF(AJ17&lt;&gt;"",AJ17,0)))</f>
+        <f>IF(X17="","",IF(OR(AN17="Received",AK17="Cleared",AN17="Refund Completed"),0,X17-IF(AJ17&lt;&gt;"",AJ17,0)))</f>
         <v/>
       </c>
       <c r="AM17" s="13" t="n"/>
@@ -3107,7 +3107,7 @@
       <c r="AJ18" s="13" t="n"/>
       <c r="AK18" s="11" t="n"/>
       <c r="AL18" s="13">
-        <f>IF(X18="","",IF(OR(AN18="Received",AK18="Cleared"),0,X18-IF(AJ18&lt;&gt;"",AJ18,0)))</f>
+        <f>IF(X18="","",IF(OR(AN18="Received",AK18="Cleared",AN18="Refund Completed"),0,X18-IF(AJ18&lt;&gt;"",AJ18,0)))</f>
         <v/>
       </c>
       <c r="AM18" s="13" t="n"/>
@@ -3171,7 +3171,7 @@
       <c r="AJ19" s="13" t="n"/>
       <c r="AK19" s="11" t="n"/>
       <c r="AL19" s="13">
-        <f>IF(X19="","",IF(OR(AN19="Received",AK19="Cleared"),0,X19-IF(AJ19&lt;&gt;"",AJ19,0)))</f>
+        <f>IF(X19="","",IF(OR(AN19="Received",AK19="Cleared",AN19="Refund Completed"),0,X19-IF(AJ19&lt;&gt;"",AJ19,0)))</f>
         <v/>
       </c>
       <c r="AM19" s="13" t="n"/>
@@ -3235,7 +3235,7 @@
       <c r="AJ20" s="13" t="n"/>
       <c r="AK20" s="11" t="n"/>
       <c r="AL20" s="13">
-        <f>IF(X20="","",IF(OR(AN20="Received",AK20="Cleared"),0,X20-IF(AJ20&lt;&gt;"",AJ20,0)))</f>
+        <f>IF(X20="","",IF(OR(AN20="Received",AK20="Cleared",AN20="Refund Completed"),0,X20-IF(AJ20&lt;&gt;"",AJ20,0)))</f>
         <v/>
       </c>
       <c r="AM20" s="13" t="n"/>
@@ -3299,7 +3299,7 @@
       <c r="AJ21" s="13" t="n"/>
       <c r="AK21" s="11" t="n"/>
       <c r="AL21" s="13">
-        <f>IF(X21="","",IF(OR(AN21="Received",AK21="Cleared"),0,X21-IF(AJ21&lt;&gt;"",AJ21,0)))</f>
+        <f>IF(X21="","",IF(OR(AN21="Received",AK21="Cleared",AN21="Refund Completed"),0,X21-IF(AJ21&lt;&gt;"",AJ21,0)))</f>
         <v/>
       </c>
       <c r="AM21" s="13" t="n"/>
@@ -3363,7 +3363,7 @@
       <c r="AJ22" s="13" t="n"/>
       <c r="AK22" s="11" t="n"/>
       <c r="AL22" s="13">
-        <f>IF(X22="","",IF(OR(AN22="Received",AK22="Cleared"),0,X22-IF(AJ22&lt;&gt;"",AJ22,0)))</f>
+        <f>IF(X22="","",IF(OR(AN22="Received",AK22="Cleared",AN22="Refund Completed"),0,X22-IF(AJ22&lt;&gt;"",AJ22,0)))</f>
         <v/>
       </c>
       <c r="AM22" s="13" t="n"/>
@@ -3427,7 +3427,7 @@
       <c r="AJ23" s="13" t="n"/>
       <c r="AK23" s="11" t="n"/>
       <c r="AL23" s="13">
-        <f>IF(X23="","",IF(OR(AN23="Received",AK23="Cleared"),0,X23-IF(AJ23&lt;&gt;"",AJ23,0)))</f>
+        <f>IF(X23="","",IF(OR(AN23="Received",AK23="Cleared",AN23="Refund Completed"),0,X23-IF(AJ23&lt;&gt;"",AJ23,0)))</f>
         <v/>
       </c>
       <c r="AM23" s="13" t="n"/>
@@ -3491,7 +3491,7 @@
       <c r="AJ24" s="13" t="n"/>
       <c r="AK24" s="11" t="n"/>
       <c r="AL24" s="13">
-        <f>IF(X24="","",IF(OR(AN24="Received",AK24="Cleared"),0,X24-IF(AJ24&lt;&gt;"",AJ24,0)))</f>
+        <f>IF(X24="","",IF(OR(AN24="Received",AK24="Cleared",AN24="Refund Completed"),0,X24-IF(AJ24&lt;&gt;"",AJ24,0)))</f>
         <v/>
       </c>
       <c r="AM24" s="13" t="n"/>
@@ -3555,7 +3555,7 @@
       <c r="AJ25" s="13" t="n"/>
       <c r="AK25" s="11" t="n"/>
       <c r="AL25" s="13">
-        <f>IF(X25="","",IF(OR(AN25="Received",AK25="Cleared"),0,X25-IF(AJ25&lt;&gt;"",AJ25,0)))</f>
+        <f>IF(X25="","",IF(OR(AN25="Received",AK25="Cleared",AN25="Refund Completed"),0,X25-IF(AJ25&lt;&gt;"",AJ25,0)))</f>
         <v/>
       </c>
       <c r="AM25" s="13" t="n"/>
@@ -3619,7 +3619,7 @@
       <c r="AJ26" s="13" t="n"/>
       <c r="AK26" s="11" t="n"/>
       <c r="AL26" s="13">
-        <f>IF(X26="","",IF(OR(AN26="Received",AK26="Cleared"),0,X26-IF(AJ26&lt;&gt;"",AJ26,0)))</f>
+        <f>IF(X26="","",IF(OR(AN26="Received",AK26="Cleared",AN26="Refund Completed"),0,X26-IF(AJ26&lt;&gt;"",AJ26,0)))</f>
         <v/>
       </c>
       <c r="AM26" s="13" t="n"/>
@@ -3683,7 +3683,7 @@
       <c r="AJ27" s="13" t="n"/>
       <c r="AK27" s="11" t="n"/>
       <c r="AL27" s="13">
-        <f>IF(X27="","",IF(OR(AN27="Received",AK27="Cleared"),0,X27-IF(AJ27&lt;&gt;"",AJ27,0)))</f>
+        <f>IF(X27="","",IF(OR(AN27="Received",AK27="Cleared",AN27="Refund Completed"),0,X27-IF(AJ27&lt;&gt;"",AJ27,0)))</f>
         <v/>
       </c>
       <c r="AM27" s="13" t="n"/>
@@ -3747,7 +3747,7 @@
       <c r="AJ28" s="13" t="n"/>
       <c r="AK28" s="11" t="n"/>
       <c r="AL28" s="13">
-        <f>IF(X28="","",IF(OR(AN28="Received",AK28="Cleared"),0,X28-IF(AJ28&lt;&gt;"",AJ28,0)))</f>
+        <f>IF(X28="","",IF(OR(AN28="Received",AK28="Cleared",AN28="Refund Completed"),0,X28-IF(AJ28&lt;&gt;"",AJ28,0)))</f>
         <v/>
       </c>
       <c r="AM28" s="13" t="n"/>
@@ -3811,7 +3811,7 @@
       <c r="AJ29" s="13" t="n"/>
       <c r="AK29" s="11" t="n"/>
       <c r="AL29" s="13">
-        <f>IF(X29="","",IF(OR(AN29="Received",AK29="Cleared"),0,X29-IF(AJ29&lt;&gt;"",AJ29,0)))</f>
+        <f>IF(X29="","",IF(OR(AN29="Received",AK29="Cleared",AN29="Refund Completed"),0,X29-IF(AJ29&lt;&gt;"",AJ29,0)))</f>
         <v/>
       </c>
       <c r="AM29" s="13" t="n"/>
@@ -3875,7 +3875,7 @@
       <c r="AJ30" s="13" t="n"/>
       <c r="AK30" s="11" t="n"/>
       <c r="AL30" s="13">
-        <f>IF(X30="","",IF(OR(AN30="Received",AK30="Cleared"),0,X30-IF(AJ30&lt;&gt;"",AJ30,0)))</f>
+        <f>IF(X30="","",IF(OR(AN30="Received",AK30="Cleared",AN30="Refund Completed"),0,X30-IF(AJ30&lt;&gt;"",AJ30,0)))</f>
         <v/>
       </c>
       <c r="AM30" s="13" t="n"/>
@@ -3939,7 +3939,7 @@
       <c r="AJ31" s="13" t="n"/>
       <c r="AK31" s="11" t="n"/>
       <c r="AL31" s="13">
-        <f>IF(X31="","",IF(OR(AN31="Received",AK31="Cleared"),0,X31-IF(AJ31&lt;&gt;"",AJ31,0)))</f>
+        <f>IF(X31="","",IF(OR(AN31="Received",AK31="Cleared",AN31="Refund Completed"),0,X31-IF(AJ31&lt;&gt;"",AJ31,0)))</f>
         <v/>
       </c>
       <c r="AM31" s="13" t="n"/>
@@ -4003,7 +4003,7 @@
       <c r="AJ32" s="13" t="n"/>
       <c r="AK32" s="11" t="n"/>
       <c r="AL32" s="13">
-        <f>IF(X32="","",IF(OR(AN32="Received",AK32="Cleared"),0,X32-IF(AJ32&lt;&gt;"",AJ32,0)))</f>
+        <f>IF(X32="","",IF(OR(AN32="Received",AK32="Cleared",AN32="Refund Completed"),0,X32-IF(AJ32&lt;&gt;"",AJ32,0)))</f>
         <v/>
       </c>
       <c r="AM32" s="13" t="n"/>
@@ -4067,7 +4067,7 @@
       <c r="AJ33" s="13" t="n"/>
       <c r="AK33" s="11" t="n"/>
       <c r="AL33" s="13">
-        <f>IF(X33="","",IF(OR(AN33="Received",AK33="Cleared"),0,X33-IF(AJ33&lt;&gt;"",AJ33,0)))</f>
+        <f>IF(X33="","",IF(OR(AN33="Received",AK33="Cleared",AN33="Refund Completed"),0,X33-IF(AJ33&lt;&gt;"",AJ33,0)))</f>
         <v/>
       </c>
       <c r="AM33" s="13" t="n"/>
@@ -4131,7 +4131,7 @@
       <c r="AJ34" s="13" t="n"/>
       <c r="AK34" s="11" t="n"/>
       <c r="AL34" s="13">
-        <f>IF(X34="","",IF(OR(AN34="Received",AK34="Cleared"),0,X34-IF(AJ34&lt;&gt;"",AJ34,0)))</f>
+        <f>IF(X34="","",IF(OR(AN34="Received",AK34="Cleared",AN34="Refund Completed"),0,X34-IF(AJ34&lt;&gt;"",AJ34,0)))</f>
         <v/>
       </c>
       <c r="AM34" s="13" t="n"/>
@@ -4195,7 +4195,7 @@
       <c r="AJ35" s="13" t="n"/>
       <c r="AK35" s="11" t="n"/>
       <c r="AL35" s="13">
-        <f>IF(X35="","",IF(OR(AN35="Received",AK35="Cleared"),0,X35-IF(AJ35&lt;&gt;"",AJ35,0)))</f>
+        <f>IF(X35="","",IF(OR(AN35="Received",AK35="Cleared",AN35="Refund Completed"),0,X35-IF(AJ35&lt;&gt;"",AJ35,0)))</f>
         <v/>
       </c>
       <c r="AM35" s="13" t="n"/>
@@ -4259,7 +4259,7 @@
       <c r="AJ36" s="13" t="n"/>
       <c r="AK36" s="11" t="n"/>
       <c r="AL36" s="13">
-        <f>IF(X36="","",IF(OR(AN36="Received",AK36="Cleared"),0,X36-IF(AJ36&lt;&gt;"",AJ36,0)))</f>
+        <f>IF(X36="","",IF(OR(AN36="Received",AK36="Cleared",AN36="Refund Completed"),0,X36-IF(AJ36&lt;&gt;"",AJ36,0)))</f>
         <v/>
       </c>
       <c r="AM36" s="13" t="n"/>
@@ -4323,7 +4323,7 @@
       <c r="AJ37" s="13" t="n"/>
       <c r="AK37" s="11" t="n"/>
       <c r="AL37" s="13">
-        <f>IF(X37="","",IF(OR(AN37="Received",AK37="Cleared"),0,X37-IF(AJ37&lt;&gt;"",AJ37,0)))</f>
+        <f>IF(X37="","",IF(OR(AN37="Received",AK37="Cleared",AN37="Refund Completed"),0,X37-IF(AJ37&lt;&gt;"",AJ37,0)))</f>
         <v/>
       </c>
       <c r="AM37" s="13" t="n"/>
@@ -4387,7 +4387,7 @@
       <c r="AJ38" s="13" t="n"/>
       <c r="AK38" s="11" t="n"/>
       <c r="AL38" s="13">
-        <f>IF(X38="","",IF(OR(AN38="Received",AK38="Cleared"),0,X38-IF(AJ38&lt;&gt;"",AJ38,0)))</f>
+        <f>IF(X38="","",IF(OR(AN38="Received",AK38="Cleared",AN38="Refund Completed"),0,X38-IF(AJ38&lt;&gt;"",AJ38,0)))</f>
         <v/>
       </c>
       <c r="AM38" s="13" t="n"/>
@@ -4451,7 +4451,7 @@
       <c r="AJ39" s="13" t="n"/>
       <c r="AK39" s="11" t="n"/>
       <c r="AL39" s="13">
-        <f>IF(X39="","",IF(OR(AN39="Received",AK39="Cleared"),0,X39-IF(AJ39&lt;&gt;"",AJ39,0)))</f>
+        <f>IF(X39="","",IF(OR(AN39="Received",AK39="Cleared",AN39="Refund Completed"),0,X39-IF(AJ39&lt;&gt;"",AJ39,0)))</f>
         <v/>
       </c>
       <c r="AM39" s="13" t="n"/>
@@ -4515,7 +4515,7 @@
       <c r="AJ40" s="13" t="n"/>
       <c r="AK40" s="11" t="n"/>
       <c r="AL40" s="13">
-        <f>IF(X40="","",IF(OR(AN40="Received",AK40="Cleared"),0,X40-IF(AJ40&lt;&gt;"",AJ40,0)))</f>
+        <f>IF(X40="","",IF(OR(AN40="Received",AK40="Cleared",AN40="Refund Completed"),0,X40-IF(AJ40&lt;&gt;"",AJ40,0)))</f>
         <v/>
       </c>
       <c r="AM40" s="13" t="n"/>
@@ -4579,7 +4579,7 @@
       <c r="AJ41" s="13" t="n"/>
       <c r="AK41" s="11" t="n"/>
       <c r="AL41" s="13">
-        <f>IF(X41="","",IF(OR(AN41="Received",AK41="Cleared"),0,X41-IF(AJ41&lt;&gt;"",AJ41,0)))</f>
+        <f>IF(X41="","",IF(OR(AN41="Received",AK41="Cleared",AN41="Refund Completed"),0,X41-IF(AJ41&lt;&gt;"",AJ41,0)))</f>
         <v/>
       </c>
       <c r="AM41" s="13" t="n"/>
@@ -4643,7 +4643,7 @@
       <c r="AJ42" s="13" t="n"/>
       <c r="AK42" s="11" t="n"/>
       <c r="AL42" s="13">
-        <f>IF(X42="","",IF(OR(AN42="Received",AK42="Cleared"),0,X42-IF(AJ42&lt;&gt;"",AJ42,0)))</f>
+        <f>IF(X42="","",IF(OR(AN42="Received",AK42="Cleared",AN42="Refund Completed"),0,X42-IF(AJ42&lt;&gt;"",AJ42,0)))</f>
         <v/>
       </c>
       <c r="AM42" s="13" t="n"/>
@@ -4707,7 +4707,7 @@
       <c r="AJ43" s="13" t="n"/>
       <c r="AK43" s="11" t="n"/>
       <c r="AL43" s="13">
-        <f>IF(X43="","",IF(OR(AN43="Received",AK43="Cleared"),0,X43-IF(AJ43&lt;&gt;"",AJ43,0)))</f>
+        <f>IF(X43="","",IF(OR(AN43="Received",AK43="Cleared",AN43="Refund Completed"),0,X43-IF(AJ43&lt;&gt;"",AJ43,0)))</f>
         <v/>
       </c>
       <c r="AM43" s="13" t="n"/>
@@ -4771,7 +4771,7 @@
       <c r="AJ44" s="13" t="n"/>
       <c r="AK44" s="11" t="n"/>
       <c r="AL44" s="13">
-        <f>IF(X44="","",IF(OR(AN44="Received",AK44="Cleared"),0,X44-IF(AJ44&lt;&gt;"",AJ44,0)))</f>
+        <f>IF(X44="","",IF(OR(AN44="Received",AK44="Cleared",AN44="Refund Completed"),0,X44-IF(AJ44&lt;&gt;"",AJ44,0)))</f>
         <v/>
       </c>
       <c r="AM44" s="13" t="n"/>
@@ -4835,7 +4835,7 @@
       <c r="AJ45" s="13" t="n"/>
       <c r="AK45" s="11" t="n"/>
       <c r="AL45" s="13">
-        <f>IF(X45="","",IF(OR(AN45="Received",AK45="Cleared"),0,X45-IF(AJ45&lt;&gt;"",AJ45,0)))</f>
+        <f>IF(X45="","",IF(OR(AN45="Received",AK45="Cleared",AN45="Refund Completed"),0,X45-IF(AJ45&lt;&gt;"",AJ45,0)))</f>
         <v/>
       </c>
       <c r="AM45" s="13" t="n"/>
@@ -4899,7 +4899,7 @@
       <c r="AJ46" s="13" t="n"/>
       <c r="AK46" s="11" t="n"/>
       <c r="AL46" s="13">
-        <f>IF(X46="","",IF(OR(AN46="Received",AK46="Cleared"),0,X46-IF(AJ46&lt;&gt;"",AJ46,0)))</f>
+        <f>IF(X46="","",IF(OR(AN46="Received",AK46="Cleared",AN46="Refund Completed"),0,X46-IF(AJ46&lt;&gt;"",AJ46,0)))</f>
         <v/>
       </c>
       <c r="AM46" s="13" t="n"/>
@@ -4963,7 +4963,7 @@
       <c r="AJ47" s="13" t="n"/>
       <c r="AK47" s="11" t="n"/>
       <c r="AL47" s="13">
-        <f>IF(X47="","",IF(OR(AN47="Received",AK47="Cleared"),0,X47-IF(AJ47&lt;&gt;"",AJ47,0)))</f>
+        <f>IF(X47="","",IF(OR(AN47="Received",AK47="Cleared",AN47="Refund Completed"),0,X47-IF(AJ47&lt;&gt;"",AJ47,0)))</f>
         <v/>
       </c>
       <c r="AM47" s="13" t="n"/>
@@ -5027,7 +5027,7 @@
       <c r="AJ48" s="13" t="n"/>
       <c r="AK48" s="11" t="n"/>
       <c r="AL48" s="13">
-        <f>IF(X48="","",IF(OR(AN48="Received",AK48="Cleared"),0,X48-IF(AJ48&lt;&gt;"",AJ48,0)))</f>
+        <f>IF(X48="","",IF(OR(AN48="Received",AK48="Cleared",AN48="Refund Completed"),0,X48-IF(AJ48&lt;&gt;"",AJ48,0)))</f>
         <v/>
       </c>
       <c r="AM48" s="13" t="n"/>
@@ -5091,7 +5091,7 @@
       <c r="AJ49" s="13" t="n"/>
       <c r="AK49" s="11" t="n"/>
       <c r="AL49" s="13">
-        <f>IF(X49="","",IF(OR(AN49="Received",AK49="Cleared"),0,X49-IF(AJ49&lt;&gt;"",AJ49,0)))</f>
+        <f>IF(X49="","",IF(OR(AN49="Received",AK49="Cleared",AN49="Refund Completed"),0,X49-IF(AJ49&lt;&gt;"",AJ49,0)))</f>
         <v/>
       </c>
       <c r="AM49" s="13" t="n"/>
@@ -5155,7 +5155,7 @@
       <c r="AJ50" s="13" t="n"/>
       <c r="AK50" s="11" t="n"/>
       <c r="AL50" s="13">
-        <f>IF(X50="","",IF(OR(AN50="Received",AK50="Cleared"),0,X50-IF(AJ50&lt;&gt;"",AJ50,0)))</f>
+        <f>IF(X50="","",IF(OR(AN50="Received",AK50="Cleared",AN50="Refund Completed"),0,X50-IF(AJ50&lt;&gt;"",AJ50,0)))</f>
         <v/>
       </c>
       <c r="AM50" s="13" t="n"/>
@@ -5219,7 +5219,7 @@
       <c r="AJ51" s="13" t="n"/>
       <c r="AK51" s="11" t="n"/>
       <c r="AL51" s="13">
-        <f>IF(X51="","",IF(OR(AN51="Received",AK51="Cleared"),0,X51-IF(AJ51&lt;&gt;"",AJ51,0)))</f>
+        <f>IF(X51="","",IF(OR(AN51="Received",AK51="Cleared",AN51="Refund Completed"),0,X51-IF(AJ51&lt;&gt;"",AJ51,0)))</f>
         <v/>
       </c>
       <c r="AM51" s="13" t="n"/>
@@ -5283,7 +5283,7 @@
       <c r="AJ52" s="13" t="n"/>
       <c r="AK52" s="11" t="n"/>
       <c r="AL52" s="13">
-        <f>IF(X52="","",IF(OR(AN52="Received",AK52="Cleared"),0,X52-IF(AJ52&lt;&gt;"",AJ52,0)))</f>
+        <f>IF(X52="","",IF(OR(AN52="Received",AK52="Cleared",AN52="Refund Completed"),0,X52-IF(AJ52&lt;&gt;"",AJ52,0)))</f>
         <v/>
       </c>
       <c r="AM52" s="13" t="n"/>
@@ -5347,7 +5347,7 @@
       <c r="AJ53" s="13" t="n"/>
       <c r="AK53" s="11" t="n"/>
       <c r="AL53" s="13">
-        <f>IF(X53="","",IF(OR(AN53="Received",AK53="Cleared"),0,X53-IF(AJ53&lt;&gt;"",AJ53,0)))</f>
+        <f>IF(X53="","",IF(OR(AN53="Received",AK53="Cleared",AN53="Refund Completed"),0,X53-IF(AJ53&lt;&gt;"",AJ53,0)))</f>
         <v/>
       </c>
       <c r="AM53" s="13" t="n"/>
@@ -5411,7 +5411,7 @@
       <c r="AJ54" s="13" t="n"/>
       <c r="AK54" s="11" t="n"/>
       <c r="AL54" s="13">
-        <f>IF(X54="","",IF(OR(AN54="Received",AK54="Cleared"),0,X54-IF(AJ54&lt;&gt;"",AJ54,0)))</f>
+        <f>IF(X54="","",IF(OR(AN54="Received",AK54="Cleared",AN54="Refund Completed"),0,X54-IF(AJ54&lt;&gt;"",AJ54,0)))</f>
         <v/>
       </c>
       <c r="AM54" s="13" t="n"/>
@@ -5475,7 +5475,7 @@
       <c r="AJ55" s="13" t="n"/>
       <c r="AK55" s="11" t="n"/>
       <c r="AL55" s="13">
-        <f>IF(X55="","",IF(OR(AN55="Received",AK55="Cleared"),0,X55-IF(AJ55&lt;&gt;"",AJ55,0)))</f>
+        <f>IF(X55="","",IF(OR(AN55="Received",AK55="Cleared",AN55="Refund Completed"),0,X55-IF(AJ55&lt;&gt;"",AJ55,0)))</f>
         <v/>
       </c>
       <c r="AM55" s="13" t="n"/>
@@ -5539,7 +5539,7 @@
       <c r="AJ56" s="13" t="n"/>
       <c r="AK56" s="11" t="n"/>
       <c r="AL56" s="13">
-        <f>IF(X56="","",IF(OR(AN56="Received",AK56="Cleared"),0,X56-IF(AJ56&lt;&gt;"",AJ56,0)))</f>
+        <f>IF(X56="","",IF(OR(AN56="Received",AK56="Cleared",AN56="Refund Completed"),0,X56-IF(AJ56&lt;&gt;"",AJ56,0)))</f>
         <v/>
       </c>
       <c r="AM56" s="13" t="n"/>
@@ -5603,7 +5603,7 @@
       <c r="AJ57" s="13" t="n"/>
       <c r="AK57" s="11" t="n"/>
       <c r="AL57" s="13">
-        <f>IF(X57="","",IF(OR(AN57="Received",AK57="Cleared"),0,X57-IF(AJ57&lt;&gt;"",AJ57,0)))</f>
+        <f>IF(X57="","",IF(OR(AN57="Received",AK57="Cleared",AN57="Refund Completed"),0,X57-IF(AJ57&lt;&gt;"",AJ57,0)))</f>
         <v/>
       </c>
       <c r="AM57" s="13" t="n"/>
@@ -5667,7 +5667,7 @@
       <c r="AJ58" s="13" t="n"/>
       <c r="AK58" s="11" t="n"/>
       <c r="AL58" s="13">
-        <f>IF(X58="","",IF(OR(AN58="Received",AK58="Cleared"),0,X58-IF(AJ58&lt;&gt;"",AJ58,0)))</f>
+        <f>IF(X58="","",IF(OR(AN58="Received",AK58="Cleared",AN58="Refund Completed"),0,X58-IF(AJ58&lt;&gt;"",AJ58,0)))</f>
         <v/>
       </c>
       <c r="AM58" s="13" t="n"/>
@@ -5731,7 +5731,7 @@
       <c r="AJ59" s="13" t="n"/>
       <c r="AK59" s="11" t="n"/>
       <c r="AL59" s="13">
-        <f>IF(X59="","",IF(OR(AN59="Received",AK59="Cleared"),0,X59-IF(AJ59&lt;&gt;"",AJ59,0)))</f>
+        <f>IF(X59="","",IF(OR(AN59="Received",AK59="Cleared",AN59="Refund Completed"),0,X59-IF(AJ59&lt;&gt;"",AJ59,0)))</f>
         <v/>
       </c>
       <c r="AM59" s="13" t="n"/>
@@ -5795,7 +5795,7 @@
       <c r="AJ60" s="13" t="n"/>
       <c r="AK60" s="11" t="n"/>
       <c r="AL60" s="13">
-        <f>IF(X60="","",IF(OR(AN60="Received",AK60="Cleared"),0,X60-IF(AJ60&lt;&gt;"",AJ60,0)))</f>
+        <f>IF(X60="","",IF(OR(AN60="Received",AK60="Cleared",AN60="Refund Completed"),0,X60-IF(AJ60&lt;&gt;"",AJ60,0)))</f>
         <v/>
       </c>
       <c r="AM60" s="13" t="n"/>
@@ -5859,7 +5859,7 @@
       <c r="AJ61" s="13" t="n"/>
       <c r="AK61" s="11" t="n"/>
       <c r="AL61" s="13">
-        <f>IF(X61="","",IF(OR(AN61="Received",AK61="Cleared"),0,X61-IF(AJ61&lt;&gt;"",AJ61,0)))</f>
+        <f>IF(X61="","",IF(OR(AN61="Received",AK61="Cleared",AN61="Refund Completed"),0,X61-IF(AJ61&lt;&gt;"",AJ61,0)))</f>
         <v/>
       </c>
       <c r="AM61" s="13" t="n"/>
@@ -5923,7 +5923,7 @@
       <c r="AJ62" s="13" t="n"/>
       <c r="AK62" s="11" t="n"/>
       <c r="AL62" s="13">
-        <f>IF(X62="","",IF(OR(AN62="Received",AK62="Cleared"),0,X62-IF(AJ62&lt;&gt;"",AJ62,0)))</f>
+        <f>IF(X62="","",IF(OR(AN62="Received",AK62="Cleared",AN62="Refund Completed"),0,X62-IF(AJ62&lt;&gt;"",AJ62,0)))</f>
         <v/>
       </c>
       <c r="AM62" s="13" t="n"/>
@@ -5987,7 +5987,7 @@
       <c r="AJ63" s="13" t="n"/>
       <c r="AK63" s="11" t="n"/>
       <c r="AL63" s="13">
-        <f>IF(X63="","",IF(OR(AN63="Received",AK63="Cleared"),0,X63-IF(AJ63&lt;&gt;"",AJ63,0)))</f>
+        <f>IF(X63="","",IF(OR(AN63="Received",AK63="Cleared",AN63="Refund Completed"),0,X63-IF(AJ63&lt;&gt;"",AJ63,0)))</f>
         <v/>
       </c>
       <c r="AM63" s="13" t="n"/>
@@ -6051,7 +6051,7 @@
       <c r="AJ64" s="13" t="n"/>
       <c r="AK64" s="11" t="n"/>
       <c r="AL64" s="13">
-        <f>IF(X64="","",IF(OR(AN64="Received",AK64="Cleared"),0,X64-IF(AJ64&lt;&gt;"",AJ64,0)))</f>
+        <f>IF(X64="","",IF(OR(AN64="Received",AK64="Cleared",AN64="Refund Completed"),0,X64-IF(AJ64&lt;&gt;"",AJ64,0)))</f>
         <v/>
       </c>
       <c r="AM64" s="13" t="n"/>
@@ -6115,7 +6115,7 @@
       <c r="AJ65" s="13" t="n"/>
       <c r="AK65" s="11" t="n"/>
       <c r="AL65" s="13">
-        <f>IF(X65="","",IF(OR(AN65="Received",AK65="Cleared"),0,X65-IF(AJ65&lt;&gt;"",AJ65,0)))</f>
+        <f>IF(X65="","",IF(OR(AN65="Received",AK65="Cleared",AN65="Refund Completed"),0,X65-IF(AJ65&lt;&gt;"",AJ65,0)))</f>
         <v/>
       </c>
       <c r="AM65" s="13" t="n"/>
@@ -6179,7 +6179,7 @@
       <c r="AJ66" s="13" t="n"/>
       <c r="AK66" s="11" t="n"/>
       <c r="AL66" s="13">
-        <f>IF(X66="","",IF(OR(AN66="Received",AK66="Cleared"),0,X66-IF(AJ66&lt;&gt;"",AJ66,0)))</f>
+        <f>IF(X66="","",IF(OR(AN66="Received",AK66="Cleared",AN66="Refund Completed"),0,X66-IF(AJ66&lt;&gt;"",AJ66,0)))</f>
         <v/>
       </c>
       <c r="AM66" s="13" t="n"/>
@@ -6243,7 +6243,7 @@
       <c r="AJ67" s="13" t="n"/>
       <c r="AK67" s="11" t="n"/>
       <c r="AL67" s="13">
-        <f>IF(X67="","",IF(OR(AN67="Received",AK67="Cleared"),0,X67-IF(AJ67&lt;&gt;"",AJ67,0)))</f>
+        <f>IF(X67="","",IF(OR(AN67="Received",AK67="Cleared",AN67="Refund Completed"),0,X67-IF(AJ67&lt;&gt;"",AJ67,0)))</f>
         <v/>
       </c>
       <c r="AM67" s="13" t="n"/>
@@ -6307,7 +6307,7 @@
       <c r="AJ68" s="13" t="n"/>
       <c r="AK68" s="11" t="n"/>
       <c r="AL68" s="13">
-        <f>IF(X68="","",IF(OR(AN68="Received",AK68="Cleared"),0,X68-IF(AJ68&lt;&gt;"",AJ68,0)))</f>
+        <f>IF(X68="","",IF(OR(AN68="Received",AK68="Cleared",AN68="Refund Completed"),0,X68-IF(AJ68&lt;&gt;"",AJ68,0)))</f>
         <v/>
       </c>
       <c r="AM68" s="13" t="n"/>
@@ -6371,7 +6371,7 @@
       <c r="AJ69" s="13" t="n"/>
       <c r="AK69" s="11" t="n"/>
       <c r="AL69" s="13">
-        <f>IF(X69="","",IF(OR(AN69="Received",AK69="Cleared"),0,X69-IF(AJ69&lt;&gt;"",AJ69,0)))</f>
+        <f>IF(X69="","",IF(OR(AN69="Received",AK69="Cleared",AN69="Refund Completed"),0,X69-IF(AJ69&lt;&gt;"",AJ69,0)))</f>
         <v/>
       </c>
       <c r="AM69" s="13" t="n"/>
@@ -6435,7 +6435,7 @@
       <c r="AJ70" s="13" t="n"/>
       <c r="AK70" s="11" t="n"/>
       <c r="AL70" s="13">
-        <f>IF(X70="","",IF(OR(AN70="Received",AK70="Cleared"),0,X70-IF(AJ70&lt;&gt;"",AJ70,0)))</f>
+        <f>IF(X70="","",IF(OR(AN70="Received",AK70="Cleared",AN70="Refund Completed"),0,X70-IF(AJ70&lt;&gt;"",AJ70,0)))</f>
         <v/>
       </c>
       <c r="AM70" s="13" t="n"/>
@@ -6499,7 +6499,7 @@
       <c r="AJ71" s="13" t="n"/>
       <c r="AK71" s="11" t="n"/>
       <c r="AL71" s="13">
-        <f>IF(X71="","",IF(OR(AN71="Received",AK71="Cleared"),0,X71-IF(AJ71&lt;&gt;"",AJ71,0)))</f>
+        <f>IF(X71="","",IF(OR(AN71="Received",AK71="Cleared",AN71="Refund Completed"),0,X71-IF(AJ71&lt;&gt;"",AJ71,0)))</f>
         <v/>
       </c>
       <c r="AM71" s="13" t="n"/>
@@ -6563,7 +6563,7 @@
       <c r="AJ72" s="13" t="n"/>
       <c r="AK72" s="11" t="n"/>
       <c r="AL72" s="13">
-        <f>IF(X72="","",IF(OR(AN72="Received",AK72="Cleared"),0,X72-IF(AJ72&lt;&gt;"",AJ72,0)))</f>
+        <f>IF(X72="","",IF(OR(AN72="Received",AK72="Cleared",AN72="Refund Completed"),0,X72-IF(AJ72&lt;&gt;"",AJ72,0)))</f>
         <v/>
       </c>
       <c r="AM72" s="13" t="n"/>
@@ -6627,7 +6627,7 @@
       <c r="AJ73" s="13" t="n"/>
       <c r="AK73" s="11" t="n"/>
       <c r="AL73" s="13">
-        <f>IF(X73="","",IF(OR(AN73="Received",AK73="Cleared"),0,X73-IF(AJ73&lt;&gt;"",AJ73,0)))</f>
+        <f>IF(X73="","",IF(OR(AN73="Received",AK73="Cleared",AN73="Refund Completed"),0,X73-IF(AJ73&lt;&gt;"",AJ73,0)))</f>
         <v/>
       </c>
       <c r="AM73" s="13" t="n"/>
@@ -6691,7 +6691,7 @@
       <c r="AJ74" s="13" t="n"/>
       <c r="AK74" s="11" t="n"/>
       <c r="AL74" s="13">
-        <f>IF(X74="","",IF(OR(AN74="Received",AK74="Cleared"),0,X74-IF(AJ74&lt;&gt;"",AJ74,0)))</f>
+        <f>IF(X74="","",IF(OR(AN74="Received",AK74="Cleared",AN74="Refund Completed"),0,X74-IF(AJ74&lt;&gt;"",AJ74,0)))</f>
         <v/>
       </c>
       <c r="AM74" s="13" t="n"/>
@@ -6755,7 +6755,7 @@
       <c r="AJ75" s="13" t="n"/>
       <c r="AK75" s="11" t="n"/>
       <c r="AL75" s="13">
-        <f>IF(X75="","",IF(OR(AN75="Received",AK75="Cleared"),0,X75-IF(AJ75&lt;&gt;"",AJ75,0)))</f>
+        <f>IF(X75="","",IF(OR(AN75="Received",AK75="Cleared",AN75="Refund Completed"),0,X75-IF(AJ75&lt;&gt;"",AJ75,0)))</f>
         <v/>
       </c>
       <c r="AM75" s="13" t="n"/>
@@ -6819,7 +6819,7 @@
       <c r="AJ76" s="13" t="n"/>
       <c r="AK76" s="11" t="n"/>
       <c r="AL76" s="13">
-        <f>IF(X76="","",IF(OR(AN76="Received",AK76="Cleared"),0,X76-IF(AJ76&lt;&gt;"",AJ76,0)))</f>
+        <f>IF(X76="","",IF(OR(AN76="Received",AK76="Cleared",AN76="Refund Completed"),0,X76-IF(AJ76&lt;&gt;"",AJ76,0)))</f>
         <v/>
       </c>
       <c r="AM76" s="13" t="n"/>
@@ -6883,7 +6883,7 @@
       <c r="AJ77" s="13" t="n"/>
       <c r="AK77" s="11" t="n"/>
       <c r="AL77" s="13">
-        <f>IF(X77="","",IF(OR(AN77="Received",AK77="Cleared"),0,X77-IF(AJ77&lt;&gt;"",AJ77,0)))</f>
+        <f>IF(X77="","",IF(OR(AN77="Received",AK77="Cleared",AN77="Refund Completed"),0,X77-IF(AJ77&lt;&gt;"",AJ77,0)))</f>
         <v/>
       </c>
       <c r="AM77" s="13" t="n"/>
@@ -6947,7 +6947,7 @@
       <c r="AJ78" s="13" t="n"/>
       <c r="AK78" s="11" t="n"/>
       <c r="AL78" s="13">
-        <f>IF(X78="","",IF(OR(AN78="Received",AK78="Cleared"),0,X78-IF(AJ78&lt;&gt;"",AJ78,0)))</f>
+        <f>IF(X78="","",IF(OR(AN78="Received",AK78="Cleared",AN78="Refund Completed"),0,X78-IF(AJ78&lt;&gt;"",AJ78,0)))</f>
         <v/>
       </c>
       <c r="AM78" s="13" t="n"/>
@@ -7011,7 +7011,7 @@
       <c r="AJ79" s="13" t="n"/>
       <c r="AK79" s="11" t="n"/>
       <c r="AL79" s="13">
-        <f>IF(X79="","",IF(OR(AN79="Received",AK79="Cleared"),0,X79-IF(AJ79&lt;&gt;"",AJ79,0)))</f>
+        <f>IF(X79="","",IF(OR(AN79="Received",AK79="Cleared",AN79="Refund Completed"),0,X79-IF(AJ79&lt;&gt;"",AJ79,0)))</f>
         <v/>
       </c>
       <c r="AM79" s="13" t="n"/>
@@ -7075,7 +7075,7 @@
       <c r="AJ80" s="13" t="n"/>
       <c r="AK80" s="11" t="n"/>
       <c r="AL80" s="13">
-        <f>IF(X80="","",IF(OR(AN80="Received",AK80="Cleared"),0,X80-IF(AJ80&lt;&gt;"",AJ80,0)))</f>
+        <f>IF(X80="","",IF(OR(AN80="Received",AK80="Cleared",AN80="Refund Completed"),0,X80-IF(AJ80&lt;&gt;"",AJ80,0)))</f>
         <v/>
       </c>
       <c r="AM80" s="13" t="n"/>
@@ -7139,7 +7139,7 @@
       <c r="AJ81" s="13" t="n"/>
       <c r="AK81" s="11" t="n"/>
       <c r="AL81" s="13">
-        <f>IF(X81="","",IF(OR(AN81="Received",AK81="Cleared"),0,X81-IF(AJ81&lt;&gt;"",AJ81,0)))</f>
+        <f>IF(X81="","",IF(OR(AN81="Received",AK81="Cleared",AN81="Refund Completed"),0,X81-IF(AJ81&lt;&gt;"",AJ81,0)))</f>
         <v/>
       </c>
       <c r="AM81" s="13" t="n"/>
@@ -7203,7 +7203,7 @@
       <c r="AJ82" s="13" t="n"/>
       <c r="AK82" s="11" t="n"/>
       <c r="AL82" s="13">
-        <f>IF(X82="","",IF(OR(AN82="Received",AK82="Cleared"),0,X82-IF(AJ82&lt;&gt;"",AJ82,0)))</f>
+        <f>IF(X82="","",IF(OR(AN82="Received",AK82="Cleared",AN82="Refund Completed"),0,X82-IF(AJ82&lt;&gt;"",AJ82,0)))</f>
         <v/>
       </c>
       <c r="AM82" s="13" t="n"/>
@@ -7267,7 +7267,7 @@
       <c r="AJ83" s="13" t="n"/>
       <c r="AK83" s="11" t="n"/>
       <c r="AL83" s="13">
-        <f>IF(X83="","",IF(OR(AN83="Received",AK83="Cleared"),0,X83-IF(AJ83&lt;&gt;"",AJ83,0)))</f>
+        <f>IF(X83="","",IF(OR(AN83="Received",AK83="Cleared",AN83="Refund Completed"),0,X83-IF(AJ83&lt;&gt;"",AJ83,0)))</f>
         <v/>
       </c>
       <c r="AM83" s="13" t="n"/>
@@ -7331,7 +7331,7 @@
       <c r="AJ84" s="13" t="n"/>
       <c r="AK84" s="11" t="n"/>
       <c r="AL84" s="13">
-        <f>IF(X84="","",IF(OR(AN84="Received",AK84="Cleared"),0,X84-IF(AJ84&lt;&gt;"",AJ84,0)))</f>
+        <f>IF(X84="","",IF(OR(AN84="Received",AK84="Cleared",AN84="Refund Completed"),0,X84-IF(AJ84&lt;&gt;"",AJ84,0)))</f>
         <v/>
       </c>
       <c r="AM84" s="13" t="n"/>
@@ -7395,7 +7395,7 @@
       <c r="AJ85" s="13" t="n"/>
       <c r="AK85" s="11" t="n"/>
       <c r="AL85" s="13">
-        <f>IF(X85="","",IF(OR(AN85="Received",AK85="Cleared"),0,X85-IF(AJ85&lt;&gt;"",AJ85,0)))</f>
+        <f>IF(X85="","",IF(OR(AN85="Received",AK85="Cleared",AN85="Refund Completed"),0,X85-IF(AJ85&lt;&gt;"",AJ85,0)))</f>
         <v/>
       </c>
       <c r="AM85" s="13" t="n"/>
@@ -7459,7 +7459,7 @@
       <c r="AJ86" s="13" t="n"/>
       <c r="AK86" s="11" t="n"/>
       <c r="AL86" s="13">
-        <f>IF(X86="","",IF(OR(AN86="Received",AK86="Cleared"),0,X86-IF(AJ86&lt;&gt;"",AJ86,0)))</f>
+        <f>IF(X86="","",IF(OR(AN86="Received",AK86="Cleared",AN86="Refund Completed"),0,X86-IF(AJ86&lt;&gt;"",AJ86,0)))</f>
         <v/>
       </c>
       <c r="AM86" s="13" t="n"/>
@@ -7523,7 +7523,7 @@
       <c r="AJ87" s="13" t="n"/>
       <c r="AK87" s="11" t="n"/>
       <c r="AL87" s="13">
-        <f>IF(X87="","",IF(OR(AN87="Received",AK87="Cleared"),0,X87-IF(AJ87&lt;&gt;"",AJ87,0)))</f>
+        <f>IF(X87="","",IF(OR(AN87="Received",AK87="Cleared",AN87="Refund Completed"),0,X87-IF(AJ87&lt;&gt;"",AJ87,0)))</f>
         <v/>
       </c>
       <c r="AM87" s="13" t="n"/>
@@ -7587,7 +7587,7 @@
       <c r="AJ88" s="13" t="n"/>
       <c r="AK88" s="11" t="n"/>
       <c r="AL88" s="13">
-        <f>IF(X88="","",IF(OR(AN88="Received",AK88="Cleared"),0,X88-IF(AJ88&lt;&gt;"",AJ88,0)))</f>
+        <f>IF(X88="","",IF(OR(AN88="Received",AK88="Cleared",AN88="Refund Completed"),0,X88-IF(AJ88&lt;&gt;"",AJ88,0)))</f>
         <v/>
       </c>
       <c r="AM88" s="13" t="n"/>
@@ -7651,7 +7651,7 @@
       <c r="AJ89" s="13" t="n"/>
       <c r="AK89" s="11" t="n"/>
       <c r="AL89" s="13">
-        <f>IF(X89="","",IF(OR(AN89="Received",AK89="Cleared"),0,X89-IF(AJ89&lt;&gt;"",AJ89,0)))</f>
+        <f>IF(X89="","",IF(OR(AN89="Received",AK89="Cleared",AN89="Refund Completed"),0,X89-IF(AJ89&lt;&gt;"",AJ89,0)))</f>
         <v/>
       </c>
       <c r="AM89" s="13" t="n"/>
@@ -7715,7 +7715,7 @@
       <c r="AJ90" s="13" t="n"/>
       <c r="AK90" s="11" t="n"/>
       <c r="AL90" s="13">
-        <f>IF(X90="","",IF(OR(AN90="Received",AK90="Cleared"),0,X90-IF(AJ90&lt;&gt;"",AJ90,0)))</f>
+        <f>IF(X90="","",IF(OR(AN90="Received",AK90="Cleared",AN90="Refund Completed"),0,X90-IF(AJ90&lt;&gt;"",AJ90,0)))</f>
         <v/>
       </c>
       <c r="AM90" s="13" t="n"/>
@@ -7779,7 +7779,7 @@
       <c r="AJ91" s="13" t="n"/>
       <c r="AK91" s="11" t="n"/>
       <c r="AL91" s="13">
-        <f>IF(X91="","",IF(OR(AN91="Received",AK91="Cleared"),0,X91-IF(AJ91&lt;&gt;"",AJ91,0)))</f>
+        <f>IF(X91="","",IF(OR(AN91="Received",AK91="Cleared",AN91="Refund Completed"),0,X91-IF(AJ91&lt;&gt;"",AJ91,0)))</f>
         <v/>
       </c>
       <c r="AM91" s="13" t="n"/>
@@ -7843,7 +7843,7 @@
       <c r="AJ92" s="13" t="n"/>
       <c r="AK92" s="11" t="n"/>
       <c r="AL92" s="13">
-        <f>IF(X92="","",IF(OR(AN92="Received",AK92="Cleared"),0,X92-IF(AJ92&lt;&gt;"",AJ92,0)))</f>
+        <f>IF(X92="","",IF(OR(AN92="Received",AK92="Cleared",AN92="Refund Completed"),0,X92-IF(AJ92&lt;&gt;"",AJ92,0)))</f>
         <v/>
       </c>
       <c r="AM92" s="13" t="n"/>
@@ -7907,7 +7907,7 @@
       <c r="AJ93" s="13" t="n"/>
       <c r="AK93" s="11" t="n"/>
       <c r="AL93" s="13">
-        <f>IF(X93="","",IF(OR(AN93="Received",AK93="Cleared"),0,X93-IF(AJ93&lt;&gt;"",AJ93,0)))</f>
+        <f>IF(X93="","",IF(OR(AN93="Received",AK93="Cleared",AN93="Refund Completed"),0,X93-IF(AJ93&lt;&gt;"",AJ93,0)))</f>
         <v/>
       </c>
       <c r="AM93" s="13" t="n"/>
@@ -7971,7 +7971,7 @@
       <c r="AJ94" s="13" t="n"/>
       <c r="AK94" s="11" t="n"/>
       <c r="AL94" s="13">
-        <f>IF(X94="","",IF(OR(AN94="Received",AK94="Cleared"),0,X94-IF(AJ94&lt;&gt;"",AJ94,0)))</f>
+        <f>IF(X94="","",IF(OR(AN94="Received",AK94="Cleared",AN94="Refund Completed"),0,X94-IF(AJ94&lt;&gt;"",AJ94,0)))</f>
         <v/>
       </c>
       <c r="AM94" s="13" t="n"/>
@@ -8035,7 +8035,7 @@
       <c r="AJ95" s="13" t="n"/>
       <c r="AK95" s="11" t="n"/>
       <c r="AL95" s="13">
-        <f>IF(X95="","",IF(OR(AN95="Received",AK95="Cleared"),0,X95-IF(AJ95&lt;&gt;"",AJ95,0)))</f>
+        <f>IF(X95="","",IF(OR(AN95="Received",AK95="Cleared",AN95="Refund Completed"),0,X95-IF(AJ95&lt;&gt;"",AJ95,0)))</f>
         <v/>
       </c>
       <c r="AM95" s="13" t="n"/>
@@ -8099,7 +8099,7 @@
       <c r="AJ96" s="13" t="n"/>
       <c r="AK96" s="11" t="n"/>
       <c r="AL96" s="13">
-        <f>IF(X96="","",IF(OR(AN96="Received",AK96="Cleared"),0,X96-IF(AJ96&lt;&gt;"",AJ96,0)))</f>
+        <f>IF(X96="","",IF(OR(AN96="Received",AK96="Cleared",AN96="Refund Completed"),0,X96-IF(AJ96&lt;&gt;"",AJ96,0)))</f>
         <v/>
       </c>
       <c r="AM96" s="13" t="n"/>
@@ -8163,7 +8163,7 @@
       <c r="AJ97" s="13" t="n"/>
       <c r="AK97" s="11" t="n"/>
       <c r="AL97" s="13">
-        <f>IF(X97="","",IF(OR(AN97="Received",AK97="Cleared"),0,X97-IF(AJ97&lt;&gt;"",AJ97,0)))</f>
+        <f>IF(X97="","",IF(OR(AN97="Received",AK97="Cleared",AN97="Refund Completed"),0,X97-IF(AJ97&lt;&gt;"",AJ97,0)))</f>
         <v/>
       </c>
       <c r="AM97" s="13" t="n"/>
@@ -8227,7 +8227,7 @@
       <c r="AJ98" s="13" t="n"/>
       <c r="AK98" s="11" t="n"/>
       <c r="AL98" s="13">
-        <f>IF(X98="","",IF(OR(AN98="Received",AK98="Cleared"),0,X98-IF(AJ98&lt;&gt;"",AJ98,0)))</f>
+        <f>IF(X98="","",IF(OR(AN98="Received",AK98="Cleared",AN98="Refund Completed"),0,X98-IF(AJ98&lt;&gt;"",AJ98,0)))</f>
         <v/>
       </c>
       <c r="AM98" s="13" t="n"/>
@@ -8291,7 +8291,7 @@
       <c r="AJ99" s="13" t="n"/>
       <c r="AK99" s="11" t="n"/>
       <c r="AL99" s="13">
-        <f>IF(X99="","",IF(OR(AN99="Received",AK99="Cleared"),0,X99-IF(AJ99&lt;&gt;"",AJ99,0)))</f>
+        <f>IF(X99="","",IF(OR(AN99="Received",AK99="Cleared",AN99="Refund Completed"),0,X99-IF(AJ99&lt;&gt;"",AJ99,0)))</f>
         <v/>
       </c>
       <c r="AM99" s="13" t="n"/>
@@ -8355,7 +8355,7 @@
       <c r="AJ100" s="13" t="n"/>
       <c r="AK100" s="11" t="n"/>
       <c r="AL100" s="13">
-        <f>IF(X100="","",IF(OR(AN100="Received",AK100="Cleared"),0,X100-IF(AJ100&lt;&gt;"",AJ100,0)))</f>
+        <f>IF(X100="","",IF(OR(AN100="Received",AK100="Cleared",AN100="Refund Completed"),0,X100-IF(AJ100&lt;&gt;"",AJ100,0)))</f>
         <v/>
       </c>
       <c r="AM100" s="13" t="n"/>
@@ -8401,35 +8401,38 @@
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="2">
       <formula>"Pending"</formula>
     </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
+      <formula>"Refund Completed"</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK1000">
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="0">
       <formula>"Received"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="1">
       <formula>"NIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="6">
       <formula>"Cleared"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:AR1000">
-    <cfRule type="expression" priority="12" dxfId="7">
+    <cfRule type="expression" priority="13" dxfId="7">
       <formula>$AB4="Confirmed"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" dxfId="8">
+    <cfRule type="expression" priority="14" dxfId="8">
       <formula>$AB4="Pending"</formula>
     </cfRule>
-    <cfRule type="expression" priority="14" dxfId="9">
+    <cfRule type="expression" priority="15" dxfId="9">
       <formula>$AB4="Cancelled"</formula>
     </cfRule>
-    <cfRule type="expression" priority="15" dxfId="10">
+    <cfRule type="expression" priority="16" dxfId="10">
       <formula>$AB4="Scheduled"</formula>
     </cfRule>
-    <cfRule type="expression" priority="16" dxfId="11">
+    <cfRule type="expression" priority="17" dxfId="11">
       <formula>$AB4="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" priority="17" dxfId="12">
+    <cfRule type="expression" priority="18" dxfId="12">
       <formula>$AB4="Refunded"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8471,7 +8474,7 @@
       <formula1>"Received,NIL,Cleared"</formula1>
     </dataValidation>
     <dataValidation sqref="AN4:AN1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>"Received,Pending"</formula1>
+      <formula1>"Received,Pending,Refund Completed"</formula1>
     </dataValidation>
     <dataValidation sqref="AO4:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"Cash,UPI,Debit Card,Payment Gateway,Bank Transfer,Other"</formula1>
@@ -8686,6 +8689,11 @@
           <t>Total Refunds</t>
         </is>
       </c>
+      <c r="I11" s="6" t="inlineStr">
+        <is>
+          <t>Refund Completed</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="40" customHeight="1">
       <c r="A12" s="30">
@@ -8720,6 +8728,10 @@
         <f>SUM('Lead Tracker'!AP4:AP1000)</f>
         <v/>
       </c>
+      <c r="I12" s="31">
+        <f>COUNTIF('Lead Tracker'!AN4:AN1000,"Refund Completed")</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="22" t="inlineStr">
@@ -9897,12 +9909,12 @@
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A1:N1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Add detailed IMPORTRANGE formulas in Form Fields Reference for easy form linking
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1810,7 +1810,7 @@
         <v/>
       </c>
       <c r="B4" s="8" t="n">
-        <v>46044.78111086666</v>
+        <v>46044.81476144233</v>
       </c>
       <c r="C4" s="9">
         <f>IF(B4&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -1892,7 +1892,7 @@
         <v/>
       </c>
       <c r="Y4" s="14" t="n">
-        <v>46051.78111086666</v>
+        <v>46051.81476144233</v>
       </c>
       <c r="Z4" s="11" t="inlineStr">
         <is>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AF4" s="11" t="n"/>
       <c r="AG4" s="14" t="n">
-        <v>46051.78111086666</v>
+        <v>46051.81476144233</v>
       </c>
       <c r="AH4" s="11" t="inlineStr">
         <is>
@@ -1958,7 +1958,7 @@
         <v/>
       </c>
       <c r="B5" s="8" t="n">
-        <v>46046.78111086666</v>
+        <v>46046.81476144233</v>
       </c>
       <c r="C5" s="9">
         <f>IF(B5&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2028,7 +2028,7 @@
         <v/>
       </c>
       <c r="Y5" s="14" t="n">
-        <v>46054.78111086666</v>
+        <v>46054.81476144233</v>
       </c>
       <c r="Z5" s="11" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v/>
       </c>
       <c r="B6" s="8" t="n">
-        <v>46042.78111086666</v>
+        <v>46042.81476144233</v>
       </c>
       <c r="C6" s="9">
         <f>IF(B6&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2196,7 +2196,7 @@
         <v/>
       </c>
       <c r="B7" s="8" t="n">
-        <v>46047.78111086666</v>
+        <v>46047.81476144233</v>
       </c>
       <c r="C7" s="9">
         <f>IF(B7&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2270,7 +2270,7 @@
         <v/>
       </c>
       <c r="Y7" s="14" t="n">
-        <v>46052.78111086666</v>
+        <v>46052.81476144233</v>
       </c>
       <c r="Z7" s="11" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="AF7" s="11" t="n"/>
       <c r="AG7" s="14" t="n">
-        <v>46052.78111086666</v>
+        <v>46052.81476144233</v>
       </c>
       <c r="AH7" s="11" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
         <v/>
       </c>
       <c r="B8" s="8" t="n">
-        <v>46039.78111086666</v>
+        <v>46039.81476144233</v>
       </c>
       <c r="C8" s="9">
         <f>IF(B8&lt;&gt;"","ST-"&amp;TEXT(ROW()-3,"0000"),"")</f>
@@ -2406,7 +2406,7 @@
         <v/>
       </c>
       <c r="Y8" s="14" t="n">
-        <v>46041.78111086666</v>
+        <v>46041.81476144233</v>
       </c>
       <c r="Z8" s="11" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="AF8" s="11" t="n"/>
       <c r="AG8" s="14" t="n">
-        <v>46041.78111086666</v>
+        <v>46041.81476144233</v>
       </c>
       <c r="AH8" s="11" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="AI8" s="14" t="n">
-        <v>46041.78111086666</v>
+        <v>46041.81476144233</v>
       </c>
       <c r="AJ8" s="13" t="n">
         <v>0</v>
@@ -9930,7 +9930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10290,72 +10290,200 @@
     <row r="24" ht="22" customHeight="1">
       <c r="A24" s="49" t="inlineStr">
         <is>
-          <t>1. Create a new Google Form at forms.google.com with the fields listed above.</t>
+          <t>1. Create a Google Form at forms.google.com with the fields listed above.</t>
         </is>
       </c>
     </row>
     <row r="25" ht="22" customHeight="1">
       <c r="A25" s="49" t="inlineStr">
         <is>
-          <t>2. Go to Responses tab in the Form &gt; Click the Google Sheets icon to link responses.</t>
+          <t>2. Go to Responses tab in the Form &gt; Click the Google Sheets icon &gt; Create a new spreadsheet.</t>
         </is>
       </c>
     </row>
     <row r="26" ht="22" customHeight="1">
       <c r="A26" s="49" t="inlineStr">
         <is>
-          <t>3. A new response sheet is created automatically in Google Sheets.</t>
+          <t>3. A response sheet is created automatically. Open it and COPY THE URL from the browser bar.</t>
         </is>
       </c>
     </row>
     <row r="27" ht="22" customHeight="1">
       <c r="A27" s="49" t="inlineStr">
         <is>
-          <t>4. In the Lead Tracker sheet, use IMPORTRANGE or copy-paste data from the response sheet.</t>
+          <t>4. Open your Lead Tracker Google Sheet. Go to cell B4.</t>
         </is>
       </c>
     </row>
     <row r="28" ht="22" customHeight="1">
       <c r="A28" s="49" t="inlineStr">
         <is>
-          <t>5. Example: =IMPORTRANGE("spreadsheet_url", "Form Responses 1!A2:R100")</t>
+          <t>5. PASTE THIS EXACT FORMULA (replace YOUR_URL with the response sheet URL you copied):</t>
         </is>
       </c>
     </row>
     <row r="29" ht="22" customHeight="1">
-      <c r="A29" s="49" t="inlineStr">
-        <is>
-          <t>6. Map the form fields to the correct Lead Tracker columns (D, E, F, G, H, I, J, K, L, M, N, P, R, T, Y, Z, AA).</t>
-        </is>
-      </c>
+      <c r="A29" s="49" t="inlineStr"/>
     </row>
     <row r="30" ht="22" customHeight="1">
       <c r="A30" s="49" t="inlineStr">
         <is>
-          <t>7. The Order ID (C), S.No (A), Total Value (V), Discounted Total (X), Pending Balance (AL), and Invoice (AQ) auto-populate.</t>
+          <t>STEP-BY-STEP IMPORTRANGE FORMULAS (paste each into the Lead Tracker):</t>
         </is>
       </c>
     </row>
     <row r="31" ht="22" customHeight="1">
       <c r="A31" s="49" t="inlineStr">
         <is>
-          <t>8. Manually update: Order Status (AB), Vendor details (AD-AF), Payment info (AJ-AO), etc.</t>
+          <t>Cell B4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!A2:A")   ← Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="22" customHeight="1">
+      <c r="A32" s="49" t="inlineStr">
+        <is>
+          <t>Cell D4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!B2:B")   ← Customer Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="22" customHeight="1">
+      <c r="A33" s="49" t="inlineStr">
+        <is>
+          <t>Cell E4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!C2:C")   ← Phone Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="22" customHeight="1">
+      <c r="A34" s="49" t="inlineStr">
+        <is>
+          <t>Cell F4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!D2:D")   ← WhatsApp Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="22" customHeight="1">
+      <c r="A35" s="49" t="inlineStr">
+        <is>
+          <t>Cell H4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!E2:E")   ← Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="22" customHeight="1">
+      <c r="A36" s="49" t="inlineStr">
+        <is>
+          <t>Cell I4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!F2:F")   ← City</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="22" customHeight="1">
+      <c r="A37" s="49" t="inlineStr">
+        <is>
+          <t>Cell J4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!G2:G")   ← Area / Locality</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="22" customHeight="1">
+      <c r="A38" s="49" t="inlineStr">
+        <is>
+          <t>Cell K4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!H2:H")   ← Full Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="22" customHeight="1">
+      <c r="A39" s="49" t="inlineStr">
+        <is>
+          <t>Cell L4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!I2:I")   ← BHK</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="22" customHeight="1">
+      <c r="A40" s="49" t="inlineStr">
+        <is>
+          <t>Cell M4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!J2:J")   ← SQFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="22" customHeight="1">
+      <c r="A41" s="49" t="inlineStr">
+        <is>
+          <t>Cell N4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!K2:K")   ← Service 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="22" customHeight="1">
+      <c r="A42" s="49" t="inlineStr">
+        <is>
+          <t>Cell Y4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!L2:L")   ← Preferred Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="22" customHeight="1">
+      <c r="A43" s="49" t="inlineStr">
+        <is>
+          <t>Cell Z4:  =IMPORTRANGE("YOUR_URL","Form Responses 1!M2:M")   ← Time Slot</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="22" customHeight="1">
+      <c r="A44" s="49" t="inlineStr">
+        <is>
+          <t>Cell AA4: =IMPORTRANGE("YOUR_URL","Form Responses 1!N2:N")   ← Order Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="22" customHeight="1">
+      <c r="A45" s="49" t="inlineStr"/>
+    </row>
+    <row r="46" ht="22" customHeight="1">
+      <c r="A46" s="49" t="inlineStr">
+        <is>
+          <t>IMPORTANT: When you paste the first IMPORTRANGE, Google Sheets will ask 'Allow access?' — click ALLOW.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="22" customHeight="1">
+      <c r="A47" s="49" t="inlineStr">
+        <is>
+          <t>Auto-calculated columns (S.No, Order ID, Total Value, Discounted Total, Pending Balance, Invoice) will fill in automatically.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="22" customHeight="1">
+      <c r="A48" s="49" t="inlineStr">
+        <is>
+          <t>Manually update: Prices (O,Q,S,U), Order Status (AB), Vendor details (AD-AF), Payment info (AJ-AO), etc.</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="28">
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A45:C45"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix freeze panes - only freeze columns A-B for better scrolling
</commit_message>
<xml_diff>
--- a/Home_Services_Lead_Tracker.xlsx
+++ b/Home_Services_Lead_Tracker.xlsx
@@ -1514,7 +1514,7 @@
   <dimension ref="A1:AR100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="16" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="n">
-        <v>46044.85731156706</v>
+        <v>46044.86105053994</v>
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="L4" s="11" t="n">
-        <v>46051.85731156706</v>
+        <v>46051.86105053994</v>
       </c>
       <c r="M4" s="9" t="inlineStr">
         <is>
@@ -1922,7 +1922,7 @@
       </c>
       <c r="AF4" s="9" t="n"/>
       <c r="AG4" s="11" t="n">
-        <v>46051.85731156706</v>
+        <v>46051.86105053994</v>
       </c>
       <c r="AH4" s="9" t="inlineStr">
         <is>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="n">
-        <v>46046.85731156706</v>
+        <v>46046.86105053994</v>
       </c>
       <c r="B5" s="8" t="inlineStr">
         <is>
@@ -2001,7 +2001,7 @@
         </is>
       </c>
       <c r="L5" s="11" t="n">
-        <v>46054.85731156706</v>
+        <v>46054.86105053994</v>
       </c>
       <c r="M5" s="9" t="inlineStr">
         <is>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="n">
-        <v>46042.85731156706</v>
+        <v>46042.86105053994</v>
       </c>
       <c r="B6" s="8" t="inlineStr">
         <is>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
-        <v>46047.85731156706</v>
+        <v>46047.86105053994</v>
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="L7" s="11" t="n">
-        <v>46052.85731156706</v>
+        <v>46052.86105053994</v>
       </c>
       <c r="M7" s="9" t="inlineStr">
         <is>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="AF7" s="9" t="n"/>
       <c r="AG7" s="11" t="n">
-        <v>46052.85731156706</v>
+        <v>46052.86105053994</v>
       </c>
       <c r="AH7" s="9" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
-        <v>46039.85731156706</v>
+        <v>46039.86105053994</v>
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="L8" s="11" t="n">
-        <v>46041.85731156706</v>
+        <v>46041.86105053994</v>
       </c>
       <c r="M8" s="9" t="inlineStr">
         <is>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="AF8" s="9" t="n"/>
       <c r="AG8" s="11" t="n">
-        <v>46041.85731156706</v>
+        <v>46041.86105053994</v>
       </c>
       <c r="AH8" s="9" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="AI8" s="11" t="n">
-        <v>46041.85731156706</v>
+        <v>46041.86105053994</v>
       </c>
       <c r="AJ8" s="14" t="n">
         <v>0</v>

</xml_diff>